<commit_message>
Kleine update aan logische testen
</commit_message>
<xml_diff>
--- a/catalogusdata/Logische testen Catalogus.xlsx
+++ b/catalogusdata/Logische testen Catalogus.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$2:$G$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$2:$H$2</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
   <si>
     <t>US</t>
   </si>
@@ -58,9 +58,6 @@
     <t>Bij start test is er geen data aanwezig</t>
   </si>
   <si>
-    <t>Regressietest #1 is uitgevoerd</t>
-  </si>
-  <si>
     <t>container/concepten-put-xml</t>
   </si>
   <si>
@@ -74,6 +71,28 @@
   </si>
   <si>
     <t>Foutmelding "De upload bevat reeds bestaande concepten"</t>
+  </si>
+  <si>
+    <t>Ingelogde gebruiker</t>
+  </si>
+  <si>
+    <t>ebadmin</t>
+  </si>
+  <si>
+    <t>Testbestand is geupload</t>
+  </si>
+  <si>
+    <t>Testbestand wordt nogmaals geupload</t>
+  </si>
+  <si>
+    <t>Testbestand 1 is geupload</t>
+  </si>
+  <si>
+    <t>Testbestand 2 wordt geupload</t>
+  </si>
+  <si>
+    <t>1. Omgevingsdocumenten/Testdata Omgevingsdocument X.xml
+2. Omgevingsdocumenten/Testdata Omgevingsdocument X.xml</t>
   </si>
 </sst>
 </file>
@@ -585,13 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G405"/>
+  <dimension ref="A1:H405"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,13 +615,13 @@
     <col min="1" max="1" width="9.140625" style="15"/>
     <col min="2" max="2" width="15.28515625" style="6" customWidth="1"/>
     <col min="3" max="3" width="35.7109375" style="12" customWidth="1"/>
-    <col min="4" max="4" width="35.7109375" style="13" customWidth="1"/>
-    <col min="5" max="5" width="35.7109375" style="14" customWidth="1"/>
-    <col min="6" max="7" width="35.7109375" style="15" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="5" width="35.7109375" style="13" customWidth="1"/>
+    <col min="6" max="6" width="35.7109375" style="14" customWidth="1"/>
+    <col min="7" max="8" width="35.7109375" style="15" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
@@ -616,15 +632,16 @@
         <v>1</v>
       </c>
       <c r="D1" s="3"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="5" t="s">
+      <c r="E1" s="3"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11"/>
       <c r="B2" s="7"/>
       <c r="C2" s="8" t="s">
@@ -633,13 +650,16 @@
       <c r="D2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="11"/>
       <c r="G2" s="11"/>
-    </row>
-    <row r="3" spans="1:7" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="H2" s="11"/>
+    </row>
+    <row r="3" spans="1:8" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15">
         <v>1</v>
       </c>
@@ -652,17 +672,20 @@
       <c r="D3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="G3" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H3" s="15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <v>2</v>
       </c>
@@ -675,17 +698,20 @@
       <c r="D4" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>11</v>
+      <c r="E4" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>20</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <v>3</v>
       </c>
@@ -693,22 +719,25 @@
         <v>7</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>11</v>
+        <v>24</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>22</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <v>4</v>
       </c>
@@ -716,67 +745,70 @@
         <v>7</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="G6" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="15">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
         <v>14</v>
       </c>
@@ -2727,7 +2759,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B2:G2"/>
+  <autoFilter ref="B2:H2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
- Regressietest geupdate - Testbestanden aangemaakt / verplaatst
</commit_message>
<xml_diff>
--- a/catalogusdata/Logische testen Catalogus.xlsx
+++ b/catalogusdata/Logische testen Catalogus.xlsx
@@ -46,9 +46,6 @@
     <t>Testbestand(en)</t>
   </si>
   <si>
-    <t>Omgevingsdocumenten/Testdata Omgevingsdocument X.xml</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
@@ -59,12 +56,6 @@
   </si>
   <si>
     <t>container/concepten-put-xml</t>
-  </si>
-  <si>
-    <t>De concepten "gebouw", "bouwwerk" en "brandveilig gebruiksactiviteit" zijn zichtbaar in de Catalogus</t>
-  </si>
-  <si>
-    <t>Het concept "gebouw" is gewijzigd (ander label)</t>
   </si>
   <si>
     <t>Foutmelding "De upload bevat concepten die nog niet bestaan"</t>
@@ -85,14 +76,26 @@
     <t>Testbestand wordt nogmaals geupload</t>
   </si>
   <si>
-    <t>Testbestand 1 is geupload</t>
+    <t>- De concepten "gebouw" en "bouwwerk" zijn zichtbaar in de Catalogus
+- Beiden concepten hebben een rdfs:label, een skos:prefLabel en een skos:definition
+- "Gebouw" is een specialisatie van "bouwwerk"</t>
   </si>
   <si>
-    <t>Testbestand 2 wordt geupload</t>
+    <t>Omgevingsdocumenten/Regressietest/Regressietest #1.xml</t>
   </si>
   <si>
-    <t>1. Omgevingsdocumenten/Testdata Omgevingsdocument X.xml
-2. Omgevingsdocumenten/Testdata Omgevingsdocument X.xml</t>
+    <t>- Het concept "gebouw" is gewijzigd (het heet nu "gebouwtje")
+- Het concept "bouwwerk" is ongewijzigd (geen nieuwe versie zichtbaar)</t>
+  </si>
+  <si>
+    <t>Testbestand Regressietest #1.xml is geupload</t>
+  </si>
+  <si>
+    <t>Omgevingsdocumenten/Regressietest/Regressietest #1.xml
+Omgevingsdocumenten/Regressietest/Regressietest #3.xml</t>
+  </si>
+  <si>
+    <t>Testbestand Regressietest #3.xml wordt geupload</t>
   </si>
 </sst>
 </file>
@@ -253,7 +256,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -298,6 +301,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -607,7 +613,7 @@
   <dimension ref="A1:H405"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,7 +629,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -651,7 +657,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F2" s="10" t="s">
         <v>5</v>
@@ -659,7 +665,7 @@
       <c r="G2" s="11"/>
       <c r="H2" s="11"/>
     </row>
-    <row r="3" spans="1:8" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="120.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15">
         <v>1</v>
       </c>
@@ -670,19 +676,19 @@
         <v>6</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="E3" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="16" t="s">
         <v>19</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -696,22 +702,22 @@
         <v>6</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <v>3</v>
       </c>
@@ -719,22 +725,22 @@
         <v>7</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F5" s="14" t="s">
         <v>22</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" s="15" t="s">
-        <v>15</v>
+        <v>24</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -745,22 +751,22 @@
         <v>7</v>
       </c>
       <c r="C6" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="15" t="s">
         <v>13</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="15" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
- Kleine fix voor XML-containers - Verdere uitbreiding logische testen
</commit_message>
<xml_diff>
--- a/catalogusdata/Logische testen Catalogus.xlsx
+++ b/catalogusdata/Logische testen Catalogus.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="37">
   <si>
     <t>US</t>
   </si>
@@ -71,16 +71,10 @@
   </si>
   <si>
     <t>Omgevingsdocumenten/Regressietest/Regressietest #1.xml</t>
-  </si>
-  <si>
-    <t>Testbestand Regressietest #1.xml is geupload</t>
   </si>
   <si>
     <t>Omgevingsdocumenten/Regressietest/Regressietest #1.xml
 Omgevingsdocumenten/Regressietest/Regressietest #3.xml</t>
-  </si>
-  <si>
-    <t>Testbestand Regressietest #3.xml wordt geupload</t>
   </si>
   <si>
     <t>Container geeft als foutmelding "De upload bevat reeds bestaande concepten"</t>
@@ -128,6 +122,25 @@
     <t>Op de pagina is o.a. een tabelweergave te zien met als header 'gebouwtje' en o.a. de volgende rij:
 - Naam | Gebouwtje
 Tevens is er een tabel te zien met als kolomheaders 'Andere versies' en 'Actueel tot', met daarin één rij met een link en een niet-lege waarde.</t>
+  </si>
+  <si>
+    <t>Omgevingsdocumenten/Regressietest/Regressietest #8.xml</t>
+  </si>
+  <si>
+    <t>Container geeft als foutmelding "De upload mag geen concepten of collecties zonder term bevatten."</t>
+  </si>
+  <si>
+    <t>Omgevingsdocumenten/Regressietest/Regressietest #1.xml
+Omgevingsdocumenten/Regressietest/Regressietest #8.xml</t>
+  </si>
+  <si>
+    <t>Testbestand #1 is geupload</t>
+  </si>
+  <si>
+    <t>Testbestand #3 wordt geupload</t>
+  </si>
+  <si>
+    <t>Testbestand #8 wordt geupload</t>
   </si>
 </sst>
 </file>
@@ -644,14 +657,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H405"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="15"/>
-    <col min="2" max="2" width="15.28515625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="3.85546875" style="15" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" style="6" customWidth="1"/>
     <col min="3" max="3" width="35.7109375" style="12" customWidth="1"/>
     <col min="4" max="5" width="35.7109375" style="13" customWidth="1"/>
     <col min="6" max="6" width="35.7109375" style="14" customWidth="1"/>
@@ -720,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -746,7 +757,7 @@
         <v>16</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -760,19 +771,19 @@
         <v>12</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>14</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="G5" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" s="16" t="s">
         <v>20</v>
-      </c>
-      <c r="H5" s="16" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -798,7 +809,7 @@
         <v>10</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="180" x14ac:dyDescent="0.25">
@@ -806,7 +817,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>6</v>
@@ -815,16 +826,16 @@
         <v>17</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F7" s="14" t="s">
         <v>15</v>
       </c>
       <c r="G7" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="15" t="s">
         <v>27</v>
-      </c>
-      <c r="H7" s="15" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="168.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -832,7 +843,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>6</v>
@@ -841,16 +852,16 @@
         <v>17</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F8" s="14" t="s">
         <v>15</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="135" x14ac:dyDescent="0.25">
@@ -858,35 +869,77 @@
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="15">
         <v>9</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fix voor relatiecontrole kenniskluis
</commit_message>
<xml_diff>
--- a/catalogusdata/Logische testen Catalogus.xlsx
+++ b/catalogusdata/Logische testen Catalogus.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="55">
   <si>
     <t>US</t>
   </si>
@@ -141,6 +141,74 @@
   </si>
   <si>
     <t>Testbestand #8 wordt geupload</t>
+  </si>
+  <si>
+    <t>GCO-4</t>
+  </si>
+  <si>
+    <t>container/ttlupdate</t>
+  </si>
+  <si>
+    <t>Omgevingsdocumenten/Regressietest/Regressietest #10.xml</t>
+  </si>
+  <si>
+    <t>Omgevingsdocumenten/Regressietest/Regressietest #11.xml</t>
+  </si>
+  <si>
+    <t>Omgevingsdocumenten/Regressietest/Regressietest #12.xml</t>
+  </si>
+  <si>
+    <t>Omgevingsdocumenten/Regressietest/Regressietest #13.xml</t>
+  </si>
+  <si>
+    <t>Pagina /id/concept/GeneriekBeest wordt bekeken</t>
+  </si>
+  <si>
+    <t>Op de pagina is o.a. het volgende te zien:
+- Tabelweergave met als header 'Generiek beest'
+- Grafische weergave (leeg)
+In de tabel staan de volgende rijen (header | waarde):
+- Naam | GeneriekBeest
+- Startdatum versie | (niet leeg)
+- Laatste activiteit | (link)
+- Notitie | Notitie
+- Uitleg | Uitleg
+- Definitie | Definitie
+- Toelichting | Toelichting
+- Domein | (link)
+- Synoniemen | (link)</t>
+  </si>
+  <si>
+    <t>Testbestand #10 is geupload</t>
+  </si>
+  <si>
+    <t>Testbestand #11 is geupload</t>
+  </si>
+  <si>
+    <t>Relaties</t>
+  </si>
+  <si>
+    <t>Testbestand #12 is geupload</t>
+  </si>
+  <si>
+    <t>Testbestand #13 is geupload</t>
+  </si>
+  <si>
+    <t>Bron</t>
+  </si>
+  <si>
+    <t>GCO-294</t>
+  </si>
+  <si>
+    <t>Toeleidingsbegrippen</t>
+  </si>
+  <si>
+    <t>Pagina /query/search?term=monster wordt bekeken</t>
+  </si>
+  <si>
+    <t>Op de pagina is o.a. een tabel te zien met als headers 'concept' en 'uitleg' en daaronder één rij met daarin:
+- in de linkerkolom een link naar /id/concept/GeneriekBeest met als label 'Generiek beest'
+- in de rechterkolom de tekst "Definitie"</t>
   </si>
 </sst>
 </file>
@@ -657,7 +725,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H405"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D14" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -942,29 +1012,134 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="255" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="H12" s="15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="H14" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="H15" s="15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
         <v>14</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="H16" s="15" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
- Matrix toegevoegd - Activiteiten weggehaald uit configuratie (GCO-280)
</commit_message>
<xml_diff>
--- a/catalogusdata/Logische testen Catalogus.xlsx
+++ b/catalogusdata/Logische testen Catalogus.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="69">
   <si>
     <t>US</t>
   </si>
@@ -141,18 +141,6 @@
   </si>
   <si>
     <t>container/ttlupdate</t>
-  </si>
-  <si>
-    <t>Omgevingsdocumenten/Regressietest/Regressietest #10.xml</t>
-  </si>
-  <si>
-    <t>Omgevingsdocumenten/Regressietest/Regressietest #11.xml</t>
-  </si>
-  <si>
-    <t>Omgevingsdocumenten/Regressietest/Regressietest #12.xml</t>
-  </si>
-  <si>
-    <t>Omgevingsdocumenten/Regressietest/Regressietest #13.xml</t>
   </si>
   <si>
     <t>Pagina /id/concept/GeneriekBeest wordt bekeken</t>
@@ -245,6 +233,24 @@
   </si>
   <si>
     <t>Datacontrole toeleidingsbegrip</t>
+  </si>
+  <si>
+    <t>Zoekpagina</t>
+  </si>
+  <si>
+    <t>Toeleidingsbegrip</t>
+  </si>
+  <si>
+    <t>Omgevingsdocumenten/Regressietest/Datacontrole attributen.ttl</t>
+  </si>
+  <si>
+    <t>Omgevingsdocumenten/Regressietest/Datacontrole relaties.ttl</t>
+  </si>
+  <si>
+    <t>Omgevingsdocumenten/Regressietest/Datacontrole bron.ttl</t>
+  </si>
+  <si>
+    <t>Omgevingsdocumenten/Regressietest/Datacontrole toeleidingsbegrip.ttl</t>
   </si>
 </sst>
 </file>
@@ -764,8 +770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J405"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="D14" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,7 +788,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -805,10 +811,10 @@
         <v>9</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>0</v>
@@ -833,10 +839,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>7</v>
@@ -862,10 +868,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>7</v>
@@ -894,10 +900,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>7</v>
@@ -926,10 +932,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>7</v>
@@ -955,10 +961,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>20</v>
@@ -987,10 +993,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>58</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>62</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>24</v>
@@ -1019,10 +1025,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>20</v>
@@ -1051,10 +1057,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>20</v>
@@ -1080,10 +1086,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>63</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>20</v>
@@ -1112,10 +1118,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>35</v>
@@ -1124,19 +1130,19 @@
         <v>36</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1144,10 +1150,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>35</v>
@@ -1156,19 +1162,19 @@
         <v>36</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="G13" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="I13" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="J13" s="10" t="s">
         <v>41</v>
-      </c>
-      <c r="J13" s="10" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1176,10 +1182,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>35</v>
@@ -1188,19 +1194,19 @@
         <v>36</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="G14" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1208,57 +1214,63 @@
         <v>13</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>36</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="G15" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>14</v>
       </c>
+      <c r="B16" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>64</v>
+      </c>
       <c r="D16" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>36</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="G16" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H16" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="I16" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="I16" s="10" t="s">
-        <v>51</v>
-      </c>
       <c r="J16" s="10" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Naamgeving testbestanden Catalogus op orde gemaakt
</commit_message>
<xml_diff>
--- a/catalogusdata/Logische testen Catalogus.xlsx
+++ b/catalogusdata/Logische testen Catalogus.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="75">
   <si>
     <t>US</t>
   </si>
@@ -64,13 +64,6 @@
     <t>Testbestand wordt nogmaals geupload</t>
   </si>
   <si>
-    <t>Omgevingsdocumenten/Regressietest/Regressietest #1.xml</t>
-  </si>
-  <si>
-    <t>Omgevingsdocumenten/Regressietest/Regressietest #1.xml
-Omgevingsdocumenten/Regressietest/Regressietest #3.xml</t>
-  </si>
-  <si>
     <t>Container geeft als foutmelding "De upload bevat reeds bestaande concepten"</t>
   </si>
   <si>
@@ -86,55 +79,10 @@
     <t>-</t>
   </si>
   <si>
-    <t>Pagina /id/concept/Gebouw wordt bekeken</t>
-  </si>
-  <si>
-    <t>Pagina /id/concept/Bouwwerk wordt bekeken</t>
-  </si>
-  <si>
     <t>GCO-391</t>
   </si>
   <si>
-    <t>Op de pagina is o.a. het volgende te zien:
-- Tabelweergave met als header 'bouwwerk'
-- Grafische weergave (niet leeg)
-In de tabel staan de volgende rijen (header | waarde):
-- Naam | Bouwwerk
-- Definitie | (niet leeg)
-- Startdatum versie | (niet leeg)
-- Laatste activiteit | (link)</t>
-  </si>
-  <si>
-    <t>Op de pagina is o.a. een tabelweergave te zien met daarin o.a.:
-- Een rij met als header 'Definitie' en als waarde een stuk tekst die begint met een link met als url /id/concept/Bouwwerk en als label 'bouwwerk'
-- Een rij met als header 'Is specialisatie van' en als waarde een link met als url /id/concept/Bouwwerk en als label 'bouwwerk'</t>
-  </si>
-  <si>
-    <t>Eerst is testbestand #1 geupload, vervolgens is testbestand #3 geupload</t>
-  </si>
-  <si>
-    <t>Op de pagina is o.a. een tabelweergave te zien met als header 'gebouwtje' en o.a. de volgende rij:
-- Naam | Gebouwtje
-Tevens is er een tabel te zien met als kolomheaders 'Andere versies' en 'Actueel tot', met daarin één rij met een link en een niet-lege waarde.</t>
-  </si>
-  <si>
-    <t>Omgevingsdocumenten/Regressietest/Regressietest #8.xml</t>
-  </si>
-  <si>
     <t>Container geeft als foutmelding "De upload mag geen concepten of collecties zonder term bevatten."</t>
-  </si>
-  <si>
-    <t>Omgevingsdocumenten/Regressietest/Regressietest #1.xml
-Omgevingsdocumenten/Regressietest/Regressietest #8.xml</t>
-  </si>
-  <si>
-    <t>Testbestand #1 is geupload</t>
-  </si>
-  <si>
-    <t>Testbestand #3 wordt geupload</t>
-  </si>
-  <si>
-    <t>Testbestand #8 wordt geupload</t>
   </si>
   <si>
     <t>GCO-4</t>
@@ -161,19 +109,7 @@
 - Synoniemen | (link)</t>
   </si>
   <si>
-    <t>Testbestand #10 is geupload</t>
-  </si>
-  <si>
-    <t>Testbestand #11 is geupload</t>
-  </si>
-  <si>
     <t>Relaties</t>
-  </si>
-  <si>
-    <t>Testbestand #12 is geupload</t>
-  </si>
-  <si>
-    <t>Testbestand #13 is geupload</t>
   </si>
   <si>
     <t>Bron</t>
@@ -202,21 +138,9 @@
     <t>LOGISCHE TEST</t>
   </si>
   <si>
-    <t>Succesvolle upload</t>
-  </si>
-  <si>
     <t>Validatie bestaand concept</t>
   </si>
   <si>
-    <t>API POST XML</t>
-  </si>
-  <si>
-    <t>API PUT XML</t>
-  </si>
-  <si>
-    <t>Datacontrole</t>
-  </si>
-  <si>
     <t>Datacontrole attributen</t>
   </si>
   <si>
@@ -241,16 +165,110 @@
     <t>Toeleidingsbegrip</t>
   </si>
   <si>
-    <t>Omgevingsdocumenten/Regressietest/Datacontrole attributen.ttl</t>
-  </si>
-  <si>
-    <t>Omgevingsdocumenten/Regressietest/Datacontrole relaties.ttl</t>
-  </si>
-  <si>
-    <t>Omgevingsdocumenten/Regressietest/Datacontrole bron.ttl</t>
-  </si>
-  <si>
-    <t>Omgevingsdocumenten/Regressietest/Datacontrole toeleidingsbegrip.ttl</t>
+    <t>Concepten POST XML</t>
+  </si>
+  <si>
+    <t>Concepten PUT XML</t>
+  </si>
+  <si>
+    <t>Uploadcontrole</t>
+  </si>
+  <si>
+    <t>Datacontrole wijziging</t>
+  </si>
+  <si>
+    <t>Omgevingsdocumenten/Regressietest/Invoervalidatie.xml</t>
+  </si>
+  <si>
+    <t>Omgevingsdocumenten/Regressietest/Datacontrole relaties.xml</t>
+  </si>
+  <si>
+    <t>Omgevingsdocumenten/Regressietest/Datacontrole relaties.xml
+Omgevingsdocumenten/Regressietest/Datacontrole wijziging.xml</t>
+  </si>
+  <si>
+    <t>Testbestand is geupload</t>
+  </si>
+  <si>
+    <t>Testbestand "Datacontrole wijziging.xml" wordt geupload</t>
+  </si>
+  <si>
+    <t>Omgevingsdocumenten/Regressietest/Datacontrole attributen.xml</t>
+  </si>
+  <si>
+    <t>Omgevingsdocumenten/Regressietest/Datacontrole attributen.xml
+Omgevingsdocumenten/Regressietest/Datacontrole wijziging.xml</t>
+  </si>
+  <si>
+    <t>Omgevingsdocumenten/Regressietest/Datacontrole attributen.xml
+Omgevingsdocumenten/Regressietest/Invoervalidatie.xml</t>
+  </si>
+  <si>
+    <t>Testbestand "Datacontrole attributen.xml" is geupload</t>
+  </si>
+  <si>
+    <t>Testbestand "Invoervalidatie.xml" wordt geupload</t>
+  </si>
+  <si>
+    <t>Op de pagina is o.a. een tabelweergave te zien met daarin o.a.:
+- Een rij met als header 'Definitie' en als waarde "Definitie" plus een link met als url /id/concept/GeneriekBeest en als label 'generiek beest'
+- Een rij met als header 'Is specialisatie van' en als waarde een link met als url /id/concept/GeneriekBeest en als label 'generiek beest'</t>
+  </si>
+  <si>
+    <t>Pagina /id/concept/SpecifiekBeest wordt bekeken</t>
+  </si>
+  <si>
+    <t>Op de pagina is o.a. een tabelweergave te zien met als header 'generiek beestje' en o.a. de volgende rij:
+- Naam | GeneriekBeestje
+Tevens is er een tabel te zien met als kolomheaders 'Andere versies' en 'Actueel tot', met daarin één rij met een link en een niet-lege waarde.</t>
+  </si>
+  <si>
+    <t>Op de pagina is o.a. het volgende te zien:
+- Tabelweergave met als header 'generiek beest'
+In de tabel staan o.a. de volgende rijen (header | waarde):
+- Naam | GeneriekBeest
+- Definitie | Definitie</t>
+  </si>
+  <si>
+    <t>Volgende twee acties in onderstaande volgorde uitgevoerd:
+- Testbestand "Datacontrole attributen.xml" is geupload via /container/concepten-post-xml
+- Testbestand "Datacontrole wijziging.xml" is geupload via /container/concepten-put-xml</t>
+  </si>
+  <si>
+    <t>Testbestand "Datacontrole relaties.xml" is geupload via /container/concepten-post-xml</t>
+  </si>
+  <si>
+    <t>/query/search</t>
+  </si>
+  <si>
+    <t>Concepten/Regressietest/Datacontrole attributen.ttl</t>
+  </si>
+  <si>
+    <t>Concepten/Regressietest/Datacontrole relaties.ttl</t>
+  </si>
+  <si>
+    <t>Concepten/Regressietest/Datacontrole bron.ttl</t>
+  </si>
+  <si>
+    <t>Concepten/Regressietest/Datacontrole toeleidingsbegrip.ttl</t>
+  </si>
+  <si>
+    <t>Datacontrole collectie</t>
+  </si>
+  <si>
+    <t>Concepten/Regressietest/Datacontrole collecties.ttl</t>
+  </si>
+  <si>
+    <t>Collecties</t>
+  </si>
+  <si>
+    <t>Datacontrole waardelijsten</t>
+  </si>
+  <si>
+    <t>Concepten/Regressietest/Datacontrole waardelijsten.ttl</t>
+  </si>
+  <si>
+    <t>Waardelijsten</t>
   </si>
 </sst>
 </file>
@@ -770,8 +788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J405"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D14" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="E12" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -788,7 +806,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -811,10 +829,10 @@
         <v>9</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>0</v>
@@ -839,10 +857,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>7</v>
@@ -851,7 +869,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>13</v>
@@ -860,7 +878,7 @@
         <v>10</v>
       </c>
       <c r="J3" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -868,10 +886,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>7</v>
@@ -880,19 +898,19 @@
         <v>6</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="I4" s="10" t="s">
         <v>14</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -900,10 +918,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>7</v>
@@ -912,19 +930,19 @@
         <v>11</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -932,10 +950,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>7</v>
@@ -944,7 +962,7 @@
         <v>11</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>13</v>
@@ -953,103 +971,103 @@
         <v>10</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="180" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>5</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>6</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="I7" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="168.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="159" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>6</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>7</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>16</v>
+        <v>54</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="I9" s="10" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1057,19 +1075,19 @@
         <v>8</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>6</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>13</v>
@@ -1078,7 +1096,7 @@
         <v>10</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -1086,31 +1104,31 @@
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="G11" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="I11" s="10" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="255" x14ac:dyDescent="0.25">
@@ -1118,31 +1136,31 @@
         <v>10</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>65</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1150,31 +1168,31 @@
         <v>11</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>66</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="I13" s="10" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1182,31 +1200,31 @@
         <v>12</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>67</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1214,141 +1232,189 @@
         <v>13</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>68</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>14</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="J17" s="10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B18" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="I18" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="J18" s="10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="8">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="8">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="8">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
Regressietesten voor Concepten POST/PUT Turtle opgeleverd
</commit_message>
<xml_diff>
--- a/catalogusdata/Logische testen Catalogus.xlsx
+++ b/catalogusdata/Logische testen Catalogus.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="95">
   <si>
     <t>US</t>
   </si>
@@ -147,9 +147,6 @@
     <t>Datacontrole relaties</t>
   </si>
   <si>
-    <t>Invoervalidatie</t>
-  </si>
-  <si>
     <t>Upload Turtle</t>
   </si>
   <si>
@@ -177,14 +174,7 @@
     <t>Datacontrole wijziging</t>
   </si>
   <si>
-    <t>Omgevingsdocumenten/Regressietest/Invoervalidatie.xml</t>
-  </si>
-  <si>
     <t>Omgevingsdocumenten/Regressietest/Datacontrole relaties.xml</t>
-  </si>
-  <si>
-    <t>Omgevingsdocumenten/Regressietest/Datacontrole relaties.xml
-Omgevingsdocumenten/Regressietest/Datacontrole wijziging.xml</t>
   </si>
   <si>
     <t>Testbestand is geupload</t>
@@ -200,14 +190,7 @@
 Omgevingsdocumenten/Regressietest/Datacontrole wijziging.xml</t>
   </si>
   <si>
-    <t>Omgevingsdocumenten/Regressietest/Datacontrole attributen.xml
-Omgevingsdocumenten/Regressietest/Invoervalidatie.xml</t>
-  </si>
-  <si>
     <t>Testbestand "Datacontrole attributen.xml" is geupload</t>
-  </si>
-  <si>
-    <t>Testbestand "Invoervalidatie.xml" wordt geupload</t>
   </si>
   <si>
     <t>Op de pagina is o.a. een tabelweergave te zien met daarin o.a.:
@@ -235,40 +218,119 @@
 - Testbestand "Datacontrole wijziging.xml" is geupload via /container/concepten-put-xml</t>
   </si>
   <si>
-    <t>Testbestand "Datacontrole relaties.xml" is geupload via /container/concepten-post-xml</t>
-  </si>
-  <si>
-    <t>/query/search</t>
-  </si>
-  <si>
-    <t>Concepten/Regressietest/Datacontrole attributen.ttl</t>
-  </si>
-  <si>
-    <t>Concepten/Regressietest/Datacontrole relaties.ttl</t>
-  </si>
-  <si>
-    <t>Concepten/Regressietest/Datacontrole bron.ttl</t>
-  </si>
-  <si>
-    <t>Concepten/Regressietest/Datacontrole toeleidingsbegrip.ttl</t>
-  </si>
-  <si>
     <t>Datacontrole collectie</t>
   </si>
   <si>
-    <t>Concepten/Regressietest/Datacontrole collecties.ttl</t>
-  </si>
-  <si>
     <t>Collecties</t>
   </si>
   <si>
     <t>Datacontrole waardelijsten</t>
   </si>
   <si>
-    <t>Concepten/Regressietest/Datacontrole waardelijsten.ttl</t>
-  </si>
-  <si>
     <t>Waardelijsten</t>
+  </si>
+  <si>
+    <t>Concepten POST Turtle</t>
+  </si>
+  <si>
+    <t>GCO-470</t>
+  </si>
+  <si>
+    <t>query/search</t>
+  </si>
+  <si>
+    <t>container/concepten-post-ttl</t>
+  </si>
+  <si>
+    <t>Omgevingsdocumenten/Regressietest/Uploadcontrole.xml</t>
+  </si>
+  <si>
+    <t>Concepten PUT Turtle</t>
+  </si>
+  <si>
+    <t>container/concepten-put-ttl</t>
+  </si>
+  <si>
+    <t>Testbestand "Datacontrole wijziging.ttl" wordt geupload</t>
+  </si>
+  <si>
+    <t>Validatie term</t>
+  </si>
+  <si>
+    <t>Omgevingsdocumenten/Regressietest/Validatie term.xml</t>
+  </si>
+  <si>
+    <t>Omgevingsdocumenten/Regressietest/Datacontrole attributen.xml
+Omgevingsdocumenten/Regressietest/Validatie term.xml</t>
+  </si>
+  <si>
+    <t>Testbestand "Validatie term.xml" wordt geupload</t>
+  </si>
+  <si>
+    <t>Validatie label</t>
+  </si>
+  <si>
+    <t>Validatie prefLabel</t>
+  </si>
+  <si>
+    <t>GCO-466</t>
+  </si>
+  <si>
+    <t>Container geeft als foutmelding "De upload mag geen concepten of collecties zonder rdfs:label bevatten."</t>
+  </si>
+  <si>
+    <t>Container geeft als foutmelding "De upload mag geen concepten of collecties zonder skos:prefLabel bevatten."</t>
+  </si>
+  <si>
+    <t>Testbestand "Datacontrole attribuut.ttl" is geupload via /container/concepten-post-ttl</t>
+  </si>
+  <si>
+    <t>Testbestand "Datacontrole attributen.xml" is geupload via /container/concepten-post-xml</t>
+  </si>
+  <si>
+    <t>Testbestand "Validatie label.ttl" wordt geupload</t>
+  </si>
+  <si>
+    <t>Testbestand "Validatie prefLabel.ttl" wordt geupload</t>
+  </si>
+  <si>
+    <t>Concepten/Regressietest/ttl/Datacontrole attributen.ttl</t>
+  </si>
+  <si>
+    <t>Concepten/Regressietest/ttl/Datacontrole relaties.ttl</t>
+  </si>
+  <si>
+    <t>Concepten/Regressietest/ttl/Datacontrole bron.ttl</t>
+  </si>
+  <si>
+    <t>Concepten/Regressietest/ttl/Datacontrole toeleidingsbegrip.ttl</t>
+  </si>
+  <si>
+    <t>Concepten/Regressietest/ttl/Datacontrole collecties.ttl</t>
+  </si>
+  <si>
+    <t>Concepten/Regressietest/ttl/Datacontrole waardelijsten.ttl</t>
+  </si>
+  <si>
+    <t>Concepten/Regressietest/ttl/Uploadcontrole.ttl</t>
+  </si>
+  <si>
+    <t>Concepten/Regressietest/ttl/Validatie label.ttl</t>
+  </si>
+  <si>
+    <t>Concepten/Regressietest/ttl/Validatie prefLabel.ttl</t>
+  </si>
+  <si>
+    <t>Concepten/Regressietest/ttl/Datacontrole attribuut.ttl
+Concepten/Regressietest/ttl/Datacontrole wijziging.ttl</t>
+  </si>
+  <si>
+    <t>Concepten/Regressietest/ttl/Datacontrole attribuut.ttl
+Concepten/Regressietest/ttl/Validatie label.ttl</t>
+  </si>
+  <si>
+    <t>Concepten/Regressietest/ttl/Datacontrole attribuut.ttl
+Concepten/Regressietest/ttl/Validatie prefLabel.ttl</t>
   </si>
 </sst>
 </file>
@@ -788,8 +850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J405"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E12" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -857,10 +919,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>7</v>
@@ -869,7 +931,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>13</v>
@@ -886,7 +948,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>35</v>
@@ -898,13 +960,13 @@
         <v>6</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I4" s="10" t="s">
         <v>14</v>
@@ -918,10 +980,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>45</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>46</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>7</v>
@@ -930,16 +992,16 @@
         <v>11</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J5" s="11" t="s">
         <v>16</v>
@@ -950,7 +1012,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>35</v>
@@ -962,7 +1024,7 @@
         <v>11</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>13</v>
@@ -979,7 +1041,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>36</v>
@@ -991,19 +1053,19 @@
         <v>6</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>19</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I7" s="10" t="s">
         <v>24</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="159" customHeight="1" x14ac:dyDescent="0.25">
@@ -1011,7 +1073,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>37</v>
@@ -1023,19 +1085,19 @@
         <v>6</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>19</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -1043,10 +1105,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>18</v>
@@ -1055,19 +1117,19 @@
         <v>11</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>19</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="I9" s="10" t="s">
         <v>24</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1075,10 +1137,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>18</v>
@@ -1087,7 +1149,7 @@
         <v>6</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>13</v>
@@ -1104,10 +1166,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>18</v>
@@ -1116,16 +1178,16 @@
         <v>11</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="G11" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="I11" s="10" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="J11" s="10" t="s">
         <v>21</v>
@@ -1136,7 +1198,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>36</v>
@@ -1148,13 +1210,13 @@
         <v>23</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>19</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I12" s="10" t="s">
         <v>24</v>
@@ -1168,7 +1230,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>37</v>
@@ -1180,13 +1242,13 @@
         <v>23</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="G13" s="8" t="s">
         <v>19</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I13" s="10" t="s">
         <v>24</v>
@@ -1200,10 +1262,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>39</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>40</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>22</v>
@@ -1212,13 +1274,13 @@
         <v>23</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="G14" s="8" t="s">
         <v>19</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I14" s="10" t="s">
         <v>24</v>
@@ -1232,10 +1294,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>28</v>
@@ -1244,13 +1306,13 @@
         <v>23</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="G15" s="8" t="s">
         <v>19</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I15" s="10" t="s">
         <v>24</v>
@@ -1264,10 +1326,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>22</v>
@@ -1276,19 +1338,19 @@
         <v>23</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="G16" s="8" t="s">
         <v>19</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I16" s="10" t="s">
         <v>24</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1296,25 +1358,25 @@
         <v>15</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>23</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="G17" s="8" t="s">
         <v>19</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -1322,10 +1384,10 @@
         <v>16</v>
       </c>
       <c r="B18" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="8" t="s">
         <v>42</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>43</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>28</v>
@@ -1334,13 +1396,13 @@
         <v>64</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="G18" s="8" t="s">
         <v>19</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I18" s="10" t="s">
         <v>30</v>
@@ -1349,44 +1411,248 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I19" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J19" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="I20" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="J20" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B21" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I21" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J21" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B22" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I22" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J22" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B23" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="I23" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="J23" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B24" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I24" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J24" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B25" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="I25" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="J25" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
         <v>24</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="I26" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="J26" s="10" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Regressietesten JSON-LD containers toegevoegd
</commit_message>
<xml_diff>
--- a/catalogusdata/Logische testen Catalogus.xlsx
+++ b/catalogusdata/Logische testen Catalogus.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="109">
   <si>
     <t>US</t>
   </si>
@@ -331,6 +331,51 @@
   <si>
     <t>Concepten/Regressietest/ttl/Datacontrole attribuut.ttl
 Concepten/Regressietest/ttl/Validatie prefLabel.ttl</t>
+  </si>
+  <si>
+    <t>Concepten POST json-ld</t>
+  </si>
+  <si>
+    <t>Concepten PUT json-ld</t>
+  </si>
+  <si>
+    <t>container/concepten-post-jsonld</t>
+  </si>
+  <si>
+    <t>Concepten/Regressietest/jsonld/Uploadcontrole.jsonld</t>
+  </si>
+  <si>
+    <t>Concepten/Regressietest/jsonld/Validatie label.jsonld</t>
+  </si>
+  <si>
+    <t>Concepten/Regressietest/jsonld/Validatie prefLabel.jsonld</t>
+  </si>
+  <si>
+    <t>container/concepten-put-jsonld</t>
+  </si>
+  <si>
+    <t>Concepten/Regressietest/jsonld/Datacontrole attribuut.jsonld
+Concepten/Regressietest/jsonld/Datacontrole wijziging.jsonld</t>
+  </si>
+  <si>
+    <t>Testbestand "Datacontrole attribuut.jsonld" is geupload via /container/concepten-post-jsonld</t>
+  </si>
+  <si>
+    <t>Testbestand "Datacontrole wijziging.jsonld" wordt geupload</t>
+  </si>
+  <si>
+    <t>Concepten/Regressietest/jsonld/Datacontrole attribuut.jsonld
+Concepten/Regressietest/jsonld/Validatie label.jsonld</t>
+  </si>
+  <si>
+    <t>Testbestand "Validatie label.jsonld" wordt geupload</t>
+  </si>
+  <si>
+    <t>Concepten/Regressietest/jsonld/Datacontrole attribuut.jsonld
+Concepten/Regressietest/jsonld/Validatie prefLabel.jsonld</t>
+  </si>
+  <si>
+    <t>Testbestand "Validatie prefLabel.jsonld" wordt geupload</t>
   </si>
 </sst>
 </file>
@@ -850,8 +895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J405"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1655,112 +1700,316 @@
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B27" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I27" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J27" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B28" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H28" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="I28" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="J28" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B29" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I29" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J29" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="8">
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B30" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I30" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J30" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="8">
         <v>29</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B31" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H31" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="I31" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="J31" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="8">
         <v>30</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B32" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I32" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J32" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="8">
         <v>31</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B33" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H33" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="I33" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="J33" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" s="8">
         <v>32</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B34" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H34" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="I34" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="J34" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="8">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="8">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="8">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="8">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="8">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="8">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="8">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="8">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="8">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="8">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="8">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="8">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="8">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="8">
         <v>46</v>
       </c>

</xml_diff>

<commit_message>
Update aan Uitgangspunten en meer regressietesten toegevoegd
</commit_message>
<xml_diff>
--- a/catalogusdata/Logische testen Catalogus.xlsx
+++ b/catalogusdata/Logische testen Catalogus.xlsx
@@ -195,15 +195,6 @@
     <t>Datacontrole collectie</t>
   </si>
   <si>
-    <t>Collecties</t>
-  </si>
-  <si>
-    <t>Datacontrole waardelijsten</t>
-  </si>
-  <si>
-    <t>Waardelijsten</t>
-  </si>
-  <si>
     <t>Concepten POST Turtle</t>
   </si>
   <si>
@@ -278,9 +269,6 @@
   </si>
   <si>
     <t>Concepten/Regressietest/ttl/Datacontrole collecties.ttl</t>
-  </si>
-  <si>
-    <t>Concepten/Regressietest/ttl/Datacontrole waardelijsten.ttl</t>
   </si>
   <si>
     <t>Concepten/Regressietest/ttl/Uploadcontrole.ttl</t>
@@ -371,11 +359,24 @@
 - Een rij met als header 'Is specialisatie van' en als waarde een link met als url /id/concept/GeneriekBeest en als label 'Generiek beest'</t>
   </si>
   <si>
-    <t>GCO-293</t>
-  </si>
-  <si>
     <t>Op de pagina is o.a. een tabel te zien met als header 'Generiek beest' en o.a. de volgende rij:
 - Is ongeveer hetzelfde als | Monster</t>
+  </si>
+  <si>
+    <t>Weergavepagina concepten</t>
+  </si>
+  <si>
+    <t>Grafische weergave</t>
+  </si>
+  <si>
+    <t>id/concept/GeneriekBeest</t>
+  </si>
+  <si>
+    <t>Pagina wordt bekeken</t>
+  </si>
+  <si>
+    <t>Op de pagina is o.a. een tabel te zien met als header 'Generiek beest' en o.a. de volgende rij:
+- Lid van | (link naar /id/collection/StandaardBeesten met label 'Standaard beesten')</t>
   </si>
 </sst>
 </file>
@@ -895,8 +896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1376"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E16" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="E17" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -976,7 +977,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>13</v>
@@ -1006,7 +1007,7 @@
         <v>6</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>13</v>
@@ -1045,7 +1046,7 @@
         <v>13</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I5" s="10" t="s">
         <v>46</v>
@@ -1072,7 +1073,7 @@
         <v>11</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>13</v>
@@ -1114,7 +1115,7 @@
         <v>24</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="159" customHeight="1" x14ac:dyDescent="0.25">
@@ -1147,7 +1148,7 @@
         <v>50</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -1180,7 +1181,7 @@
         <v>24</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1192,7 +1193,7 @@
         <v>40</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>18</v>
@@ -1201,7 +1202,7 @@
         <v>6</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>13</v>
@@ -1222,7 +1223,7 @@
         <v>41</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>18</v>
@@ -1231,7 +1232,7 @@
         <v>11</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G11" s="8" t="s">
         <v>13</v>
@@ -1240,7 +1241,7 @@
         <v>49</v>
       </c>
       <c r="I11" s="10" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="J11" s="10" t="s">
         <v>21</v>
@@ -1264,7 +1265,7 @@
         <v>23</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>13</v>
@@ -1285,16 +1286,16 @@
         <v>36</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>23</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G13" s="8" t="s">
         <v>13</v>
@@ -1303,7 +1304,7 @@
         <v>10</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -1315,16 +1316,16 @@
         <v>36</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>23</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="G14" s="8" t="s">
         <v>13</v>
@@ -1333,7 +1334,7 @@
         <v>10</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="255" x14ac:dyDescent="0.25">
@@ -1342,7 +1343,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>36</v>
+        <v>103</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>34</v>
@@ -1351,10 +1352,10 @@
         <v>22</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>23</v>
+        <v>105</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G15" s="8" t="s">
         <v>19</v>
@@ -1363,7 +1364,7 @@
         <v>45</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>24</v>
+        <v>106</v>
       </c>
       <c r="J15" s="10" t="s">
         <v>25</v>
@@ -1375,7 +1376,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>36</v>
+        <v>103</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>43</v>
@@ -1384,22 +1385,22 @@
         <v>22</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>23</v>
+        <v>105</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G16" s="8" t="s">
         <v>19</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>24</v>
+        <v>106</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1408,7 +1409,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>36</v>
+        <v>103</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>35</v>
@@ -1417,10 +1418,10 @@
         <v>22</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>23</v>
+        <v>105</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G17" s="8" t="s">
         <v>19</v>
@@ -1429,7 +1430,7 @@
         <v>45</v>
       </c>
       <c r="I17" s="10" t="s">
-        <v>24</v>
+        <v>106</v>
       </c>
       <c r="J17" s="10" t="s">
         <v>26</v>
@@ -1441,7 +1442,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>36</v>
+        <v>103</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>37</v>
@@ -1450,10 +1451,10 @@
         <v>27</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>23</v>
+        <v>105</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G18" s="8" t="s">
         <v>19</v>
@@ -1462,19 +1463,19 @@
         <v>45</v>
       </c>
       <c r="I18" s="10" t="s">
-        <v>24</v>
+        <v>106</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>36</v>
+        <v>103</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>52</v>
@@ -1483,10 +1484,10 @@
         <v>22</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>23</v>
+        <v>105</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G19" s="8" t="s">
         <v>19</v>
@@ -1495,10 +1496,10 @@
         <v>45</v>
       </c>
       <c r="I19" s="10" t="s">
-        <v>24</v>
+        <v>106</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>53</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1507,19 +1508,16 @@
         <v>18</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>36</v>
+        <v>103</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>23</v>
+        <v>105</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G20" s="8" t="s">
         <v>19</v>
@@ -1527,13 +1525,16 @@
       <c r="H20" s="9" t="s">
         <v>45</v>
       </c>
+      <c r="I20" s="10" t="s">
+        <v>106</v>
+      </c>
       <c r="J20" s="10" t="s">
-        <v>55</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
-        <f t="shared" si="0"/>
+        <f>A20+1</f>
         <v>19</v>
       </c>
       <c r="B21" s="8" t="s">
@@ -1546,10 +1547,10 @@
         <v>27</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G21" s="8" t="s">
         <v>19</v>
@@ -1570,19 +1571,19 @@
         <v>20</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>42</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="G22" s="8" t="s">
         <v>13</v>
@@ -1600,19 +1601,19 @@
         <v>21</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="G23" s="8" t="s">
         <v>13</v>
@@ -1633,19 +1634,19 @@
         <v>22</v>
       </c>
       <c r="B24" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E24" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C24" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>59</v>
-      </c>
       <c r="F24" s="8" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G24" s="8" t="s">
         <v>13</v>
@@ -1654,7 +1655,7 @@
         <v>10</v>
       </c>
       <c r="J24" s="10" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -1663,19 +1664,19 @@
         <v>23</v>
       </c>
       <c r="B25" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E25" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C25" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>59</v>
-      </c>
       <c r="F25" s="8" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="G25" s="8" t="s">
         <v>13</v>
@@ -1684,7 +1685,7 @@
         <v>10</v>
       </c>
       <c r="J25" s="10" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -1693,28 +1694,28 @@
         <v>24</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>42</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G26" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H26" s="9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="I26" s="10" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="J26" s="11" t="s">
         <v>16</v>
@@ -1726,19 +1727,19 @@
         <v>25</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="G27" s="8" t="s">
         <v>13</v>
@@ -1756,31 +1757,31 @@
         <v>26</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G28" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="I28" s="10" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="J28" s="10" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -1789,31 +1790,31 @@
         <v>27</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="G29" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H29" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="I29" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="I29" s="10" t="s">
-        <v>76</v>
-      </c>
       <c r="J29" s="10" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1822,19 +1823,19 @@
         <v>28</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C30" s="8" t="s">
         <v>42</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="G30" s="8" t="s">
         <v>13</v>
@@ -1852,19 +1853,19 @@
         <v>29</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C31" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="G31" s="8" t="s">
         <v>13</v>
@@ -1885,19 +1886,19 @@
         <v>30</v>
       </c>
       <c r="B32" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="F32" s="8" t="s">
         <v>88</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="F32" s="8" t="s">
-        <v>92</v>
       </c>
       <c r="G32" s="8" t="s">
         <v>13</v>
@@ -1906,7 +1907,7 @@
         <v>10</v>
       </c>
       <c r="J32" s="10" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -1915,19 +1916,19 @@
         <v>31</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="G33" s="8" t="s">
         <v>13</v>
@@ -1936,7 +1937,7 @@
         <v>10</v>
       </c>
       <c r="J33" s="10" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -1945,28 +1946,28 @@
         <v>32</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C34" s="8" t="s">
         <v>42</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H34" s="9" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="I34" s="10" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="J34" s="11" t="s">
         <v>16</v>
@@ -1978,19 +1979,19 @@
         <v>33</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C35" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="G35" s="8" t="s">
         <v>13</v>
@@ -2008,31 +2009,31 @@
         <v>34</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E36" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="F36" s="8" t="s">
         <v>94</v>
-      </c>
-      <c r="F36" s="8" t="s">
-        <v>98</v>
       </c>
       <c r="G36" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H36" s="9" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="I36" s="10" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="J36" s="10" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2041,31 +2042,31 @@
         <v>35</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="G37" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H37" s="9" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="I37" s="10" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="J37" s="10" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Logische testen voor relaties, bron en grafische weergave
</commit_message>
<xml_diff>
--- a/catalogusdata/Logische testen Catalogus.xlsx
+++ b/catalogusdata/Logische testen Catalogus.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$D$2:$J$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$J$2</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="125">
   <si>
     <t>US</t>
   </si>
@@ -92,24 +92,6 @@
   </si>
   <si>
     <t>Pagina /id/concept/GeneriekBeest wordt bekeken</t>
-  </si>
-  <si>
-    <t>Op de pagina is o.a. het volgende te zien:
-- Tabelweergave met als header 'Generiek beest'
-- Grafische weergave (leeg)
-In de tabel staan de volgende rijen (header | waarde):
-- Naam | GeneriekBeest
-- Startdatum versie | (niet leeg)
-- Laatste activiteit | (link)
-- Notitie | Notitie
-- Uitleg | Uitleg
-- Definitie | Definitie
-- Toelichting | Toelichting
-- Domein | (link)
-- Synoniemen | (link)</t>
-  </si>
-  <si>
-    <t>Relaties</t>
   </si>
   <si>
     <t>GCO-294</t>
@@ -366,9 +348,6 @@
     <t>Weergavepagina concepten</t>
   </si>
   <si>
-    <t>Grafische weergave</t>
-  </si>
-  <si>
     <t>id/concept/GeneriekBeest</t>
   </si>
   <si>
@@ -377,6 +356,100 @@
   <si>
     <t>Op de pagina is o.a. een tabel te zien met als header 'Generiek beest' en o.a. de volgende rij:
 - Lid van | (link naar /id/collection/StandaardBeesten met label 'Standaard beesten')</t>
+  </si>
+  <si>
+    <t>Op de pagina is o.a. het volgende te zien:
+- Tabelweergave met als header 'Generiek beest'
+In de tabel staan o.a. de volgende rijen (header | waarde):
+- Naam | GeneriekBeest
+- Notitie | Notitie
+- Uitleg | Uitleg
+- Definitie | Definitie
+- Toelichting | Toelichting
+- Domein | (link naar /id/concept/BeestDomein)
+- Synoniemen | Generiek dier</t>
+  </si>
+  <si>
+    <t>Links concepten</t>
+  </si>
+  <si>
+    <t>Op de pagina is o.a. het volgende te zien:
+- Tabelweergave met als header 'Generiek beest'
+In de tabel staan de volgende rijen (header | waarde):
+- Is generalisatie van | (link naar id/concept/SpecifiekBeest met label "Specifiek beest")
+- Heeft betrekking op | (link naar id/concept/AnderBeest met label "Ander beest")
+- Bestaat uit | (link naar id/concept/Lijf met label "Lijf")
+- Is gerealiseerd in | (link naar id/concept/Focusbeest met label "Focusbeest")
+- Is hetzelfde als | (link naar id/concept/HetzelfdeBeest met label "Hetzelfde beest")
+- Zie ook (in ander schema) | (link naar id/concept/GerelateerdBeest met label "Gerelateerd beest")
+- Is breder dan (in ander schema) | (link naar id/concept/BrederBeest met label "Breder beest")
+- Is enger dan (in ander schema) | (link naar id/concept/EngerBeest met label "Enger beest")</t>
+  </si>
+  <si>
+    <t>Op de volgende link geklikt wordt:
+- id/concept/SpecifiekBeest</t>
+  </si>
+  <si>
+    <t>De weergavepagina voor SpecifiekBeest wordt geopend in hetzelfde scherm.</t>
+  </si>
+  <si>
+    <t>id/concept/NogSpecifiekerBeest</t>
+  </si>
+  <si>
+    <t>Op de pagina is o.a. een tabel te zien met als header 'Nog specifieker beest' en o.a. de volgende rij:
+- Is specialisatie van | (link naar id/concept/SpecifiekBeest met label "Specifiek beest")</t>
+  </si>
+  <si>
+    <t>id/concept/Kop</t>
+  </si>
+  <si>
+    <t>Op de pagina is o.a. een tabel te zien met als header 'Kop' en o.a. de volgende rij:
+- Is onderdeel van | (link naar id/concept/GeneriekBeest met label "Generiek beest")</t>
+  </si>
+  <si>
+    <t>Op de pagina is o.a. een grafische weergave te zien met als header 'Generiek beest'. Deze grafische weergave bevat een legenda en de volgende elementen:
+- Generiek beest
+- Specifiek beest
+- Kop
+- Lijf
+- Ander beest</t>
+  </si>
+  <si>
+    <t>Grafische weergave relaties</t>
+  </si>
+  <si>
+    <t>Grafische weergave collecties</t>
+  </si>
+  <si>
+    <t>Grafische weergave toeleidingsbegrip</t>
+  </si>
+  <si>
+    <t>Op de pagina is o.a. een grafische weergave te zien met als header 'Generiek beest'. Deze grafische weergave bevat een legenda en de volgende elementen:
+- Generiek beest
+- Standaard beesten</t>
+  </si>
+  <si>
+    <t>Op de pagina is o.a. een grafische weergave te zien met als header 'Generiek beest'. Deze grafische weergave bevat een legenda en de volgende elementen:
+- Generiek beest
+- Monster</t>
+  </si>
+  <si>
+    <t>Grafische weergave bron</t>
+  </si>
+  <si>
+    <t>Datacontrole bron</t>
+  </si>
+  <si>
+    <t>Concepten/Regressietest/ttl/Datacontrole bron.ttl</t>
+  </si>
+  <si>
+    <t>Op de pagina is o.a. een tabel te zien met als header 'Generiek beest' en o.a. de volgende rij:
+- Bron | (link naar /id/concept/Bron met label 'Bron')</t>
+  </si>
+  <si>
+    <t>Op de pagina is o.a. een grafische weergave te zien met als header 'Generiek beest'. Deze grafische weergave bevat een legenda en de volgende elementen:
+- Generiek beest
+- Bron</t>
   </si>
 </sst>
 </file>
@@ -896,8 +969,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1376"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E17" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B24" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -908,13 +984,14 @@
     <col min="5" max="5" width="35.7109375" style="7" customWidth="1"/>
     <col min="6" max="7" width="35.7109375" style="8" customWidth="1"/>
     <col min="8" max="8" width="35.7109375" style="9" customWidth="1"/>
-    <col min="9" max="10" width="35.7109375" style="10" customWidth="1"/>
+    <col min="9" max="9" width="35.7109375" style="10" customWidth="1"/>
+    <col min="10" max="10" width="71.42578125" style="10" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -937,10 +1014,10 @@
         <v>9</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>0</v>
@@ -965,10 +1042,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>40</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>42</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>7</v>
@@ -977,7 +1054,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>13</v>
@@ -995,10 +1072,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>7</v>
@@ -1007,13 +1084,13 @@
         <v>6</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I4" s="10" t="s">
         <v>14</v>
@@ -1028,10 +1105,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>7</v>
@@ -1040,16 +1117,16 @@
         <v>11</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J5" s="11" t="s">
         <v>16</v>
@@ -1061,10 +1138,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>7</v>
@@ -1073,7 +1150,7 @@
         <v>11</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>13</v>
@@ -1091,10 +1168,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>18</v>
@@ -1103,19 +1180,19 @@
         <v>6</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>19</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I7" s="10" t="s">
         <v>24</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="159" customHeight="1" x14ac:dyDescent="0.25">
@@ -1124,10 +1201,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>20</v>
@@ -1136,19 +1213,19 @@
         <v>6</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>19</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -1157,10 +1234,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>41</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>43</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>18</v>
@@ -1169,19 +1246,19 @@
         <v>11</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>19</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I9" s="10" t="s">
         <v>24</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1190,10 +1267,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>18</v>
@@ -1202,7 +1279,7 @@
         <v>6</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>13</v>
@@ -1220,10 +1297,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>18</v>
@@ -1232,16 +1309,16 @@
         <v>11</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G11" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I11" s="10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J11" s="10" t="s">
         <v>21</v>
@@ -1253,10 +1330,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>22</v>
@@ -1265,7 +1342,7 @@
         <v>23</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>13</v>
@@ -1283,19 +1360,19 @@
         <v>11</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C13" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>67</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>23</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G13" s="8" t="s">
         <v>13</v>
@@ -1304,7 +1381,7 @@
         <v>10</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -1313,19 +1390,19 @@
         <v>12</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>23</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G14" s="8" t="s">
         <v>13</v>
@@ -1334,40 +1411,40 @@
         <v>10</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="255" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="225" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G15" s="8" t="s">
         <v>19</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>25</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -1376,64 +1453,64 @@
         <v>14</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G16" s="8" t="s">
         <v>19</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="273" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G17" s="8" t="s">
         <v>19</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I17" s="10" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>26</v>
+        <v>107</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -1442,379 +1519,391 @@
         <v>16</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G18" s="8" t="s">
         <v>19</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I18" s="10" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G19" s="8" t="s">
         <v>19</v>
       </c>
       <c r="H19" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I19" s="10" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>104</v>
+        <v>35</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="G20" s="8" t="s">
         <v>19</v>
       </c>
       <c r="H20" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I20" s="10" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <f>A20+1</f>
         <v>19</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>38</v>
+        <v>101</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>55</v>
+        <v>102</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G21" s="8" t="s">
         <v>19</v>
       </c>
       <c r="H21" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I21" s="10" t="s">
-        <v>28</v>
+        <v>103</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>53</v>
+        <v>101</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>42</v>
+        <v>121</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>56</v>
+        <v>102</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>78</v>
+        <v>122</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>13</v>
+        <v>19</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>43</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="J22" s="11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+      <c r="J22" s="10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>53</v>
+        <v>101</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>33</v>
+        <v>115</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>56</v>
+        <v>102</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="H23" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I23" s="10" t="s">
-        <v>14</v>
+        <v>103</v>
       </c>
       <c r="J23" s="10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>53</v>
+        <v>101</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>65</v>
+        <v>116</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>67</v>
+        <v>22</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>56</v>
+        <v>102</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>13</v>
+        <v>19</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>43</v>
       </c>
       <c r="I24" s="10" t="s">
-        <v>10</v>
+        <v>103</v>
       </c>
       <c r="J24" s="10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>53</v>
+        <v>101</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>66</v>
+        <v>117</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>67</v>
+        <v>25</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>56</v>
+        <v>102</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>13</v>
+        <v>19</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>43</v>
       </c>
       <c r="I25" s="10" t="s">
-        <v>10</v>
+        <v>103</v>
       </c>
       <c r="J25" s="10" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>58</v>
+        <v>101</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>42</v>
+        <v>120</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>59</v>
+        <v>102</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>81</v>
+        <v>122</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="H26" s="9" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="I26" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="J26" s="11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+      <c r="J26" s="10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>58</v>
+        <v>101</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>33</v>
+        <v>106</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>59</v>
+        <v>102</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>13</v>
+        <v>19</v>
+      </c>
+      <c r="H27" s="9" t="s">
+        <v>43</v>
       </c>
       <c r="I27" s="10" t="s">
-        <v>10</v>
+        <v>108</v>
       </c>
       <c r="J27" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>67</v>
+        <v>25</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="I28" s="10" t="s">
-        <v>72</v>
+        <v>26</v>
       </c>
       <c r="J28" s="10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="G29" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H29" s="9" t="s">
-        <v>70</v>
-      </c>
       <c r="I29" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="J29" s="10" t="s">
-        <v>69</v>
+        <v>10</v>
+      </c>
+      <c r="J29" s="11" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1823,82 +1912,82 @@
         <v>28</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>84</v>
+        <v>51</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="D30" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E30" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="E30" s="7" t="s">
-        <v>86</v>
-      </c>
       <c r="F30" s="8" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="G30" s="8" t="s">
         <v>13</v>
       </c>
+      <c r="H30" s="9" t="s">
+        <v>43</v>
+      </c>
       <c r="I30" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="J30" s="11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="J30" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="8">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>84</v>
+        <v>51</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="D31" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E31" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="E31" s="7" t="s">
-        <v>86</v>
-      </c>
       <c r="F31" s="8" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="G31" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H31" s="9" t="s">
-        <v>45</v>
-      </c>
       <c r="I31" s="10" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="J31" s="10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="8">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>84</v>
+        <v>51</v>
       </c>
       <c r="C32" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="E32" s="7" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="G32" s="8" t="s">
         <v>13</v>
@@ -1907,7 +1996,7 @@
         <v>10</v>
       </c>
       <c r="J32" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -1916,91 +2005,94 @@
         <v>31</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>84</v>
+        <v>56</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="G33" s="8" t="s">
         <v>13</v>
       </c>
+      <c r="H33" s="9" t="s">
+        <v>68</v>
+      </c>
       <c r="I33" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="J33" s="10" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="J33" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="8">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>85</v>
+        <v>56</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>90</v>
+        <v>57</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H34" s="9" t="s">
-        <v>92</v>
-      </c>
       <c r="I34" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="J34" s="11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="J34" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="8">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>85</v>
+        <v>56</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>90</v>
+        <v>57</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="G35" s="8" t="s">
         <v>13</v>
       </c>
+      <c r="H35" s="9" t="s">
+        <v>68</v>
+      </c>
       <c r="I35" s="10" t="s">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="J35" s="10" t="s">
-        <v>17</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2009,106 +2101,283 @@
         <v>34</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>85</v>
+        <v>56</v>
       </c>
       <c r="C36" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="E36" s="7" t="s">
-        <v>90</v>
+        <v>57</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="G36" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H36" s="9" t="s">
-        <v>92</v>
+        <v>68</v>
       </c>
       <c r="I36" s="10" t="s">
-        <v>95</v>
+        <v>71</v>
       </c>
       <c r="J36" s="10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="8">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="B37" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="F37" s="8" t="s">
         <v>85</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="F37" s="8" t="s">
-        <v>96</v>
       </c>
       <c r="G37" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H37" s="9" t="s">
-        <v>92</v>
-      </c>
       <c r="I37" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="J37" s="10" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="J37" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="8">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B38" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H38" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="I38" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="J38" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="8">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B39" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="G39" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I39" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J39" s="10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="8">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B40" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="G40" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I40" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J40" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A41" s="8">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B41" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="G41" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H41" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="I41" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="J41" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="8">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B42" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="G42" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I42" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J42" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A43" s="8">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B43" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="G43" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H43" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="I43" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="J43" s="10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A44" s="8">
         <f t="shared" si="0"/>
         <v>42</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F44" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="G44" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H44" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="I44" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="J44" s="10" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -10104,7 +10373,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="D2:J2"/>
+  <autoFilter ref="A2:J2"/>
   <mergeCells count="2">
     <mergeCell ref="E1:H1"/>
     <mergeCell ref="A1:D1"/>

</xml_diff>

<commit_message>
Excelupdate-containers gefixed, regressietesten Excel toegevoegd inclusief testbestanden
</commit_message>
<xml_diff>
--- a/catalogusdata/Logische testen Catalogus.xlsx
+++ b/catalogusdata/Logische testen Catalogus.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="144">
   <si>
     <t>US</t>
   </si>
@@ -229,9 +229,6 @@
     <t>Container geeft als foutmelding "De upload mag geen concepten of collecties zonder skos:prefLabel bevatten."</t>
   </si>
   <si>
-    <t>Testbestand "Datacontrole attribuut.ttl" is geupload via /container/concepten-post-ttl</t>
-  </si>
-  <si>
     <t>Testbestand "Datacontrole attributen.xml" is geupload via /container/concepten-post-xml</t>
   </si>
   <si>
@@ -262,18 +259,6 @@
     <t>Concepten/Regressietest/ttl/Validatie prefLabel.ttl</t>
   </si>
   <si>
-    <t>Concepten/Regressietest/ttl/Datacontrole attribuut.ttl
-Concepten/Regressietest/ttl/Datacontrole wijziging.ttl</t>
-  </si>
-  <si>
-    <t>Concepten/Regressietest/ttl/Datacontrole attribuut.ttl
-Concepten/Regressietest/ttl/Validatie label.ttl</t>
-  </si>
-  <si>
-    <t>Concepten/Regressietest/ttl/Datacontrole attribuut.ttl
-Concepten/Regressietest/ttl/Validatie prefLabel.ttl</t>
-  </si>
-  <si>
     <t>Concepten POST json-ld</t>
   </si>
   <si>
@@ -295,25 +280,10 @@
     <t>container/concepten-put-jsonld</t>
   </si>
   <si>
-    <t>Concepten/Regressietest/jsonld/Datacontrole attribuut.jsonld
-Concepten/Regressietest/jsonld/Datacontrole wijziging.jsonld</t>
-  </si>
-  <si>
-    <t>Testbestand "Datacontrole attribuut.jsonld" is geupload via /container/concepten-post-jsonld</t>
-  </si>
-  <si>
     <t>Testbestand "Datacontrole wijziging.jsonld" wordt geupload</t>
   </si>
   <si>
-    <t>Concepten/Regressietest/jsonld/Datacontrole attribuut.jsonld
-Concepten/Regressietest/jsonld/Validatie label.jsonld</t>
-  </si>
-  <si>
     <t>Testbestand "Validatie label.jsonld" wordt geupload</t>
-  </si>
-  <si>
-    <t>Concepten/Regressietest/jsonld/Datacontrole attribuut.jsonld
-Concepten/Regressietest/jsonld/Validatie prefLabel.jsonld</t>
   </si>
   <si>
     <t>Testbestand "Validatie prefLabel.jsonld" wordt geupload</t>
@@ -450,6 +420,96 @@
     <t>Op de pagina is o.a. een grafische weergave te zien met als header 'Generiek beest'. Deze grafische weergave bevat een legenda en de volgende elementen:
 - Generiek beest
 - Bron</t>
+  </si>
+  <si>
+    <t>Concepten POST xls</t>
+  </si>
+  <si>
+    <t>Concepten PUT xls</t>
+  </si>
+  <si>
+    <t>container/concepten-post-xls</t>
+  </si>
+  <si>
+    <t>container/concepten-put-xls</t>
+  </si>
+  <si>
+    <t>Testbestand "Datacontrole wijziging.xlsx" wordt geupload</t>
+  </si>
+  <si>
+    <t>Concepten/Regressietest/xls/Uploadcontrole.xlsx</t>
+  </si>
+  <si>
+    <t>Testbestand "Validatie label.xlsx" wordt geupload</t>
+  </si>
+  <si>
+    <t>Testbestand "Validatie prefLabel.xlsx" wordt geupload</t>
+  </si>
+  <si>
+    <t>Upload Excel</t>
+  </si>
+  <si>
+    <t>container/excelupdate</t>
+  </si>
+  <si>
+    <t>Concepten/Regressietest/xls/Validatie label.xlsx</t>
+  </si>
+  <si>
+    <t>Concepten/Regressietest/xls/Validatie prefLabel.xlsx</t>
+  </si>
+  <si>
+    <t>Concepten/Regressietest/xls/Uploadcontrole.xslx</t>
+  </si>
+  <si>
+    <t>Concepten/Regressietest/xsl/Validatie label.xslx</t>
+  </si>
+  <si>
+    <t>Concepten/Regressietest/xsl/Validatie prefLabel.xlsx</t>
+  </si>
+  <si>
+    <t>Concepten/Regressietest/ttl/Datacontrole attributen.ttl
+Concepten/Regressietest/ttl/Datacontrole wijziging.ttl</t>
+  </si>
+  <si>
+    <t>Testbestand "Datacontrole attributen.ttl" is geupload via /container/concepten-post-ttl</t>
+  </si>
+  <si>
+    <t>Concepten/Regressietest/ttl/Datacontrole attributen.ttl
+Concepten/Regressietest/ttl/Validatie label.ttl</t>
+  </si>
+  <si>
+    <t>Concepten/Regressietest/ttl/Datacontrole attributen.ttl
+Concepten/Regressietest/ttl/Validatie prefLabel.ttl</t>
+  </si>
+  <si>
+    <t>Concepten/Regressietest/jsonld/Datacontrole attributen.jsonld
+Concepten/Regressietest/jsonld/Datacontrole wijziging.jsonld</t>
+  </si>
+  <si>
+    <t>Testbestand "Datacontrole attributen.jsonld" is geupload via /container/concepten-post-jsonld</t>
+  </si>
+  <si>
+    <t>Concepten/Regressietest/jsonld/Datacontrole attributen.jsonld
+Concepten/Regressietest/jsonld/Validatie label.jsonld</t>
+  </si>
+  <si>
+    <t>Concepten/Regressietest/jsonld/Datacontrole attributen.jsonld
+Concepten/Regressietest/jsonld/Validatie prefLabel.jsonld</t>
+  </si>
+  <si>
+    <t>Concepten/Regressietest/xls/Datacontrole attributen.xlsx
+Concepten/Regressietest/xls/Datacontrole wijziging.xlsx</t>
+  </si>
+  <si>
+    <t>Testbestand "Datacontrole attributen.xlsx" is geupload via /container/concepten-post-xls</t>
+  </si>
+  <si>
+    <t>Concepten/Regressietest/xls/Datacontrole attributen.xlsx
+Concepten/Regressietest/xls/Validatie label.xlsx</t>
+  </si>
+  <si>
+    <t>Concepten/Regressietest/xls/Datacontrole attributen.xlsx
+Concepten/Regressietest/xls/Validatie prefLabel.xlsx</t>
   </si>
 </sst>
 </file>
@@ -970,10 +1030,10 @@
   <dimension ref="A1:J1376"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D26" sqref="D26"/>
+      <selection pane="bottomRight" activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1123,7 +1183,7 @@
         <v>13</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I5" s="10" t="s">
         <v>44</v>
@@ -1192,7 +1252,7 @@
         <v>24</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="159" customHeight="1" x14ac:dyDescent="0.25">
@@ -1225,10 +1285,10 @@
         <v>48</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="150" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1258,7 +1318,7 @@
         <v>24</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1342,7 +1402,7 @@
         <v>23</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>13</v>
@@ -1372,7 +1432,7 @@
         <v>23</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G13" s="8" t="s">
         <v>13</v>
@@ -1402,7 +1462,7 @@
         <v>23</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G14" s="8" t="s">
         <v>13</v>
@@ -1420,7 +1480,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>32</v>
@@ -1429,10 +1489,10 @@
         <v>22</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G15" s="8" t="s">
         <v>19</v>
@@ -1441,19 +1501,19 @@
         <v>43</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="150" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>41</v>
@@ -1462,22 +1522,22 @@
         <v>22</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>79</v>
+        <v>132</v>
       </c>
       <c r="G16" s="8" t="s">
         <v>19</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="273" customHeight="1" x14ac:dyDescent="0.25">
@@ -1486,7 +1546,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>33</v>
@@ -1495,10 +1555,10 @@
         <v>22</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G17" s="8" t="s">
         <v>19</v>
@@ -1507,10 +1567,10 @@
         <v>43</v>
       </c>
       <c r="I17" s="10" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -1519,7 +1579,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>33</v>
@@ -1528,10 +1588,10 @@
         <v>22</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G18" s="8" t="s">
         <v>19</v>
@@ -1540,10 +1600,10 @@
         <v>43</v>
       </c>
       <c r="I18" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="J18" s="10" t="s">
         <v>103</v>
-      </c>
-      <c r="J18" s="10" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -1552,7 +1612,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>33</v>
@@ -1561,10 +1621,10 @@
         <v>22</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G19" s="8" t="s">
         <v>19</v>
@@ -1573,10 +1633,10 @@
         <v>43</v>
       </c>
       <c r="I19" s="10" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1585,7 +1645,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>35</v>
@@ -1594,10 +1654,10 @@
         <v>25</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G20" s="8" t="s">
         <v>19</v>
@@ -1606,10 +1666,10 @@
         <v>43</v>
       </c>
       <c r="I20" s="10" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -1618,7 +1678,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>50</v>
@@ -1627,10 +1687,10 @@
         <v>22</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G21" s="8" t="s">
         <v>19</v>
@@ -1639,10 +1699,10 @@
         <v>43</v>
       </c>
       <c r="I21" s="10" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1651,19 +1711,19 @@
         <v>20</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="G22" s="8" t="s">
         <v>19</v>
@@ -1672,10 +1732,10 @@
         <v>43</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="J22" s="10" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -1684,19 +1744,19 @@
         <v>21</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G23" s="8" t="s">
         <v>19</v>
@@ -1705,10 +1765,10 @@
         <v>43</v>
       </c>
       <c r="I23" s="10" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="J23" s="10" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -1717,19 +1777,19 @@
         <v>22</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G24" s="8" t="s">
         <v>19</v>
@@ -1738,10 +1798,10 @@
         <v>43</v>
       </c>
       <c r="I24" s="10" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="J24" s="10" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -1750,19 +1810,19 @@
         <v>23</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>25</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G25" s="8" t="s">
         <v>19</v>
@@ -1771,10 +1831,10 @@
         <v>43</v>
       </c>
       <c r="I25" s="10" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="J25" s="10" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -1783,19 +1843,19 @@
         <v>24</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="G26" s="8" t="s">
         <v>19</v>
@@ -1804,10 +1864,10 @@
         <v>43</v>
       </c>
       <c r="I26" s="10" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="J26" s="10" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1816,19 +1876,19 @@
         <v>25</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G27" s="8" t="s">
         <v>19</v>
@@ -1837,10 +1897,10 @@
         <v>43</v>
       </c>
       <c r="I27" s="10" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="J27" s="10" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -1861,7 +1921,7 @@
         <v>53</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G28" s="8" t="s">
         <v>19</v>
@@ -1894,7 +1954,7 @@
         <v>54</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G29" s="8" t="s">
         <v>13</v>
@@ -1924,7 +1984,7 @@
         <v>54</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G30" s="8" t="s">
         <v>13</v>
@@ -1957,7 +2017,7 @@
         <v>54</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G31" s="8" t="s">
         <v>13</v>
@@ -1987,7 +2047,7 @@
         <v>54</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G32" s="8" t="s">
         <v>13</v>
@@ -2017,13 +2077,13 @@
         <v>57</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>79</v>
+        <v>132</v>
       </c>
       <c r="G33" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H33" s="9" t="s">
-        <v>68</v>
+        <v>133</v>
       </c>
       <c r="I33" s="10" t="s">
         <v>58</v>
@@ -2050,7 +2110,7 @@
         <v>57</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>13</v>
@@ -2080,16 +2140,16 @@
         <v>57</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>80</v>
+        <v>134</v>
       </c>
       <c r="G35" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H35" s="9" t="s">
-        <v>68</v>
+        <v>133</v>
       </c>
       <c r="I35" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J35" s="10" t="s">
         <v>66</v>
@@ -2113,16 +2173,16 @@
         <v>57</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>81</v>
+        <v>135</v>
       </c>
       <c r="G36" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H36" s="9" t="s">
-        <v>68</v>
+        <v>133</v>
       </c>
       <c r="I36" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J36" s="10" t="s">
         <v>67</v>
@@ -2134,7 +2194,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C37" s="8" t="s">
         <v>40</v>
@@ -2143,10 +2203,10 @@
         <v>52</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G37" s="8" t="s">
         <v>13</v>
@@ -2164,7 +2224,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C38" s="8" t="s">
         <v>31</v>
@@ -2173,10 +2233,10 @@
         <v>52</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G38" s="8" t="s">
         <v>13</v>
@@ -2197,7 +2257,7 @@
         <v>37</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C39" s="8" t="s">
         <v>63</v>
@@ -2206,10 +2266,10 @@
         <v>65</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G39" s="8" t="s">
         <v>13</v>
@@ -2227,7 +2287,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C40" s="8" t="s">
         <v>64</v>
@@ -2236,10 +2296,10 @@
         <v>65</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="G40" s="8" t="s">
         <v>13</v>
@@ -2257,7 +2317,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C41" s="8" t="s">
         <v>40</v>
@@ -2266,19 +2326,19 @@
         <v>52</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>89</v>
+        <v>136</v>
       </c>
       <c r="G41" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H41" s="9" t="s">
-        <v>90</v>
+        <v>137</v>
       </c>
       <c r="I41" s="10" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="J41" s="11" t="s">
         <v>16</v>
@@ -2290,7 +2350,7 @@
         <v>40</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C42" s="8" t="s">
         <v>31</v>
@@ -2299,10 +2359,10 @@
         <v>52</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G42" s="8" t="s">
         <v>13</v>
@@ -2320,7 +2380,7 @@
         <v>41</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C43" s="8" t="s">
         <v>63</v>
@@ -2329,19 +2389,19 @@
         <v>65</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>92</v>
+        <v>138</v>
       </c>
       <c r="G43" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H43" s="9" t="s">
-        <v>90</v>
+        <v>137</v>
       </c>
       <c r="I43" s="10" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="J43" s="10" t="s">
         <v>66</v>
@@ -2353,7 +2413,7 @@
         <v>42</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C44" s="8" t="s">
         <v>64</v>
@@ -2362,139 +2422,415 @@
         <v>65</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>94</v>
+        <v>139</v>
       </c>
       <c r="G44" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H44" s="9" t="s">
-        <v>90</v>
+        <v>137</v>
       </c>
       <c r="I44" s="10" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="J44" s="10" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="8">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B45" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="F45" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="G45" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I45" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J45" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="8">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B46" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="G46" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H46" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="I46" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="J46" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="8">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B47" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="G47" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I47" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J47" s="10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="8">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B48" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="F48" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="G48" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I48" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J48" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A49" s="8">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B49" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="F49" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="G49" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H49" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="I49" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="J49" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="8">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B50" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="F50" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="G50" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I50" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J50" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A51" s="8">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B51" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="F51" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="G51" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H51" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="I51" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="J51" s="10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A52" s="8">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B52" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E52" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="F52" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="G52" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H52" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="I52" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="J52" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="8">
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B53" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="F53" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="G53" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I53" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J53" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="8">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B54" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E54" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="F54" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="G54" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I54" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J54" s="10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="8">
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B55" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E55" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="F55" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="G55" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I55" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J55" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="8">
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="8">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="8">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="8">
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="8">
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="8">
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="8">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="8">
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="8">
         <f t="shared" si="0"/>
         <v>62</v>

</xml_diff>

<commit_message>
Samenvoeging bestanden Wessel en Lars
</commit_message>
<xml_diff>
--- a/catalogusdata/Logische testen Catalogus.xlsx
+++ b/catalogusdata/Logische testen Catalogus.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="168">
   <si>
     <t>US</t>
   </si>
@@ -510,6 +510,90 @@
   <si>
     <t>Concepten/Regressietest/xls/Datacontrole attributen.xlsx
 Concepten/Regressietest/xls/Validatie prefLabel.xlsx</t>
+  </si>
+  <si>
+    <t>Upload controle</t>
+  </si>
+  <si>
+    <t>GCO-540</t>
+  </si>
+  <si>
+    <t>container/datasetupload</t>
+  </si>
+  <si>
+    <t>DSO catalogus T.ttl</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testbestand wordt geupload </t>
+  </si>
+  <si>
+    <t>Op de pagina is o.a. het volgende te zien:
+- Tabelweergave met als header 'Test Catalogus'
+In de tabel staan o.a. de volgende rijen (header | waarde):
+- Titel | Test Catalogus
+- Beschrijving | Een Catalogus voor Testdoeleinden</t>
+  </si>
+  <si>
+    <t>GCO-526</t>
+  </si>
+  <si>
+    <t>Dataset T.ttl</t>
+  </si>
+  <si>
+    <t>Op de pagina is o.a. het volgende te zien:
+- Tabelweergave
+In de tabel staat o.a. de volgende rij (header | waarde):
+- dataset | Testdataset
+- uitleg | Een Dataset voor Testdoeleinden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Synchronisatie Controle </t>
+  </si>
+  <si>
+    <t>TestConcepten.ttl</t>
+  </si>
+  <si>
+    <t>id/catalogus/Test</t>
+  </si>
+  <si>
+    <t>Upload Catalogusinformatie</t>
+  </si>
+  <si>
+    <t>Weergavepagina Catalogus</t>
+  </si>
+  <si>
+    <t>Upload datasetinformatie</t>
+  </si>
+  <si>
+    <t>Overzichtspagina datasets</t>
+  </si>
+  <si>
+    <t>Weergavepagina datasets</t>
+  </si>
+  <si>
+    <t>query/overzichtdatasets</t>
+  </si>
+  <si>
+    <t>id/dataset/Testdataset</t>
+  </si>
+  <si>
+    <t>Op de pagina is o.a. het volgende te zien:
+- Tabelweergave met als titel "Testdataset";
+Daarnaast is er zichtbaar:
+- Titel | Testdataset
+- Beschrijving | Dataset voor testdoeleinde</t>
+  </si>
+  <si>
+    <t>update/syncttlupload</t>
+  </si>
+  <si>
+    <t>Op de pagina is een uploadcontainer zichtbaar waar uit een selectieformulier de Testdataset geselecteerd kan worden</t>
+  </si>
+  <si>
+    <t>Sync Turtleupload</t>
   </si>
 </sst>
 </file>
@@ -1030,10 +1114,10 @@
   <dimension ref="A1:J1376"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B57" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F35" sqref="F35"/>
+      <selection pane="bottomRight" activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2787,11 +2871,65 @@
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B56" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E56" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="F56" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="G56" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H56" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="I56" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="J56" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A57" s="8">
         <f t="shared" si="0"/>
         <v>55</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E57" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="F57" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="G57" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H57" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="I57" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="J57" s="10" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
@@ -2799,23 +2937,131 @@
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B58" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="C58" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E58" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="F58" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="G58" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H58" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="I58" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J58" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A59" s="8">
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B59" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E59" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="F59" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="G59" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H59" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="I59" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="J59" s="10" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A60" s="8">
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B60" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E60" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="F60" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="G60" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H60" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="I60" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="J60" s="10" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="8">
         <f t="shared" si="0"/>
         <v>59</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E61" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="F61" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="G61" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H61" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="I61" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="J61" s="10" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Validaties lege labels toegevoegd voor Catalogus
</commit_message>
<xml_diff>
--- a/catalogusdata/Logische testen Catalogus.xlsx
+++ b/catalogusdata/Logische testen Catalogus.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="172">
   <si>
     <t>US</t>
   </si>
@@ -221,12 +221,6 @@
   </si>
   <si>
     <t>GCO-466</t>
-  </si>
-  <si>
-    <t>Container geeft als foutmelding "De upload mag geen concepten of collecties zonder rdfs:label bevatten."</t>
-  </si>
-  <si>
-    <t>Container geeft als foutmelding "De upload mag geen concepten of collecties zonder skos:prefLabel bevatten."</t>
   </si>
   <si>
     <t>Testbestand "Datacontrole attributen.xml" is geupload via /container/concepten-post-xml</t>
@@ -594,6 +588,24 @@
   </si>
   <si>
     <t>Sync Turtleupload</t>
+  </si>
+  <si>
+    <t>Validatie leeg label</t>
+  </si>
+  <si>
+    <t>Validatie leeg prefLabel</t>
+  </si>
+  <si>
+    <t>Concepten/Regressietest/ttl/Validatie leeg label.ttl</t>
+  </si>
+  <si>
+    <t>Concepten/Regressietest/ttl/Validatie leeg prefLabel.ttl</t>
+  </si>
+  <si>
+    <t>Container geeft als foutmelding "De upload mag geen concepten of collecties zonder of met leeg rdfs:label bevatten."</t>
+  </si>
+  <si>
+    <t>Container geeft als foutmelding "De upload mag geen concepten of collecties zonder of met leeg skos:prefLabel bevatten."</t>
   </si>
 </sst>
 </file>
@@ -1114,10 +1126,10 @@
   <dimension ref="A1:J1376"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B57" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B62" sqref="B62"/>
+      <selection pane="bottomRight" activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1267,7 +1279,7 @@
         <v>13</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I5" s="10" t="s">
         <v>44</v>
@@ -1336,7 +1348,7 @@
         <v>24</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="159" customHeight="1" x14ac:dyDescent="0.25">
@@ -1369,7 +1381,7 @@
         <v>48</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -1402,7 +1414,7 @@
         <v>24</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1486,7 +1498,7 @@
         <v>23</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>13</v>
@@ -1498,7 +1510,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1516,7 +1528,7 @@
         <v>23</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G13" s="8" t="s">
         <v>13</v>
@@ -1525,10 +1537,10 @@
         <v>10</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1546,7 +1558,7 @@
         <v>23</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G14" s="8" t="s">
         <v>13</v>
@@ -1555,7 +1567,7 @@
         <v>10</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>67</v>
+        <v>171</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="225" x14ac:dyDescent="0.25">
@@ -1564,7 +1576,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>32</v>
@@ -1573,10 +1585,10 @@
         <v>22</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G15" s="8" t="s">
         <v>19</v>
@@ -1585,10 +1597,10 @@
         <v>43</v>
       </c>
       <c r="I15" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="J15" s="10" t="s">
         <v>95</v>
-      </c>
-      <c r="J15" s="10" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -1597,7 +1609,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>41</v>
@@ -1606,22 +1618,22 @@
         <v>22</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G16" s="8" t="s">
         <v>19</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="273" customHeight="1" x14ac:dyDescent="0.25">
@@ -1630,7 +1642,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>33</v>
@@ -1639,10 +1651,10 @@
         <v>22</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G17" s="8" t="s">
         <v>19</v>
@@ -1651,10 +1663,10 @@
         <v>43</v>
       </c>
       <c r="I17" s="10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -1663,7 +1675,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>33</v>
@@ -1672,10 +1684,10 @@
         <v>22</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G18" s="8" t="s">
         <v>19</v>
@@ -1684,10 +1696,10 @@
         <v>43</v>
       </c>
       <c r="I18" s="10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -1696,7 +1708,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>33</v>
@@ -1705,10 +1717,10 @@
         <v>22</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G19" s="8" t="s">
         <v>19</v>
@@ -1717,10 +1729,10 @@
         <v>43</v>
       </c>
       <c r="I19" s="10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1729,7 +1741,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>35</v>
@@ -1738,10 +1750,10 @@
         <v>25</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G20" s="8" t="s">
         <v>19</v>
@@ -1750,10 +1762,10 @@
         <v>43</v>
       </c>
       <c r="I20" s="10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -1762,7 +1774,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>50</v>
@@ -1771,10 +1783,10 @@
         <v>22</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G21" s="8" t="s">
         <v>19</v>
@@ -1783,10 +1795,10 @@
         <v>43</v>
       </c>
       <c r="I21" s="10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1795,19 +1807,19 @@
         <v>20</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G22" s="8" t="s">
         <v>19</v>
@@ -1816,10 +1828,10 @@
         <v>43</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J22" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -1828,19 +1840,19 @@
         <v>21</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G23" s="8" t="s">
         <v>19</v>
@@ -1849,10 +1861,10 @@
         <v>43</v>
       </c>
       <c r="I23" s="10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J23" s="10" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -1861,19 +1873,19 @@
         <v>22</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G24" s="8" t="s">
         <v>19</v>
@@ -1882,10 +1894,10 @@
         <v>43</v>
       </c>
       <c r="I24" s="10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J24" s="10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -1894,19 +1906,19 @@
         <v>23</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>25</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G25" s="8" t="s">
         <v>19</v>
@@ -1915,10 +1927,10 @@
         <v>43</v>
       </c>
       <c r="I25" s="10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J25" s="10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -1927,19 +1939,19 @@
         <v>24</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G26" s="8" t="s">
         <v>19</v>
@@ -1948,10 +1960,10 @@
         <v>43</v>
       </c>
       <c r="I26" s="10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J26" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1960,19 +1972,19 @@
         <v>25</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G27" s="8" t="s">
         <v>19</v>
@@ -1981,10 +1993,10 @@
         <v>43</v>
       </c>
       <c r="I27" s="10" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J27" s="10" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2005,7 +2017,7 @@
         <v>53</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G28" s="8" t="s">
         <v>19</v>
@@ -2038,7 +2050,7 @@
         <v>54</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G29" s="8" t="s">
         <v>13</v>
@@ -2068,7 +2080,7 @@
         <v>54</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G30" s="8" t="s">
         <v>13</v>
@@ -2101,7 +2113,7 @@
         <v>54</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G31" s="8" t="s">
         <v>13</v>
@@ -2110,7 +2122,7 @@
         <v>10</v>
       </c>
       <c r="J31" s="10" t="s">
-        <v>66</v>
+        <v>170</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2131,7 +2143,7 @@
         <v>54</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G32" s="8" t="s">
         <v>13</v>
@@ -2140,7 +2152,7 @@
         <v>10</v>
       </c>
       <c r="J32" s="10" t="s">
-        <v>67</v>
+        <v>171</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2161,13 +2173,13 @@
         <v>57</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G33" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H33" s="9" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="I33" s="10" t="s">
         <v>58</v>
@@ -2194,7 +2206,7 @@
         <v>57</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>13</v>
@@ -2224,19 +2236,19 @@
         <v>57</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G35" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H35" s="9" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="I35" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J35" s="10" t="s">
-        <v>66</v>
+        <v>170</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2257,19 +2269,19 @@
         <v>57</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G36" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H36" s="9" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="I36" s="10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J36" s="10" t="s">
-        <v>67</v>
+        <v>171</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2278,7 +2290,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C37" s="8" t="s">
         <v>40</v>
@@ -2287,10 +2299,10 @@
         <v>52</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G37" s="8" t="s">
         <v>13</v>
@@ -2308,7 +2320,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C38" s="8" t="s">
         <v>31</v>
@@ -2317,10 +2329,10 @@
         <v>52</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G38" s="8" t="s">
         <v>13</v>
@@ -2341,7 +2353,7 @@
         <v>37</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C39" s="8" t="s">
         <v>63</v>
@@ -2350,10 +2362,10 @@
         <v>65</v>
       </c>
       <c r="E39" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F39" s="8" t="s">
         <v>80</v>
-      </c>
-      <c r="F39" s="8" t="s">
-        <v>82</v>
       </c>
       <c r="G39" s="8" t="s">
         <v>13</v>
@@ -2362,7 +2374,7 @@
         <v>10</v>
       </c>
       <c r="J39" s="10" t="s">
-        <v>66</v>
+        <v>170</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2371,7 +2383,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C40" s="8" t="s">
         <v>64</v>
@@ -2380,10 +2392,10 @@
         <v>65</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G40" s="8" t="s">
         <v>13</v>
@@ -2392,7 +2404,7 @@
         <v>10</v>
       </c>
       <c r="J40" s="10" t="s">
-        <v>67</v>
+        <v>171</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2401,7 +2413,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C41" s="8" t="s">
         <v>40</v>
@@ -2410,19 +2422,19 @@
         <v>52</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G41" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H41" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="I41" s="10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J41" s="11" t="s">
         <v>16</v>
@@ -2434,7 +2446,7 @@
         <v>40</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C42" s="8" t="s">
         <v>31</v>
@@ -2443,10 +2455,10 @@
         <v>52</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G42" s="8" t="s">
         <v>13</v>
@@ -2464,7 +2476,7 @@
         <v>41</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C43" s="8" t="s">
         <v>63</v>
@@ -2473,22 +2485,22 @@
         <v>65</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G43" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H43" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="I43" s="10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J43" s="10" t="s">
-        <v>66</v>
+        <v>170</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2497,7 +2509,7 @@
         <v>42</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C44" s="8" t="s">
         <v>64</v>
@@ -2506,22 +2518,22 @@
         <v>65</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G44" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H44" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="I44" s="10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J44" s="10" t="s">
-        <v>67</v>
+        <v>171</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2530,7 +2542,7 @@
         <v>43</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C45" s="8" t="s">
         <v>40</v>
@@ -2539,10 +2551,10 @@
         <v>52</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G45" s="8" t="s">
         <v>13</v>
@@ -2560,7 +2572,7 @@
         <v>44</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C46" s="8" t="s">
         <v>31</v>
@@ -2569,10 +2581,10 @@
         <v>52</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F46" s="8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G46" s="8" t="s">
         <v>13</v>
@@ -2593,7 +2605,7 @@
         <v>45</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C47" s="8" t="s">
         <v>63</v>
@@ -2602,10 +2614,10 @@
         <v>65</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G47" s="8" t="s">
         <v>13</v>
@@ -2614,7 +2626,7 @@
         <v>10</v>
       </c>
       <c r="J47" s="10" t="s">
-        <v>66</v>
+        <v>170</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2623,7 +2635,7 @@
         <v>46</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C48" s="8" t="s">
         <v>64</v>
@@ -2632,10 +2644,10 @@
         <v>65</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F48" s="8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G48" s="8" t="s">
         <v>13</v>
@@ -2644,7 +2656,7 @@
         <v>10</v>
       </c>
       <c r="J48" s="10" t="s">
-        <v>67</v>
+        <v>171</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2653,7 +2665,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C49" s="8" t="s">
         <v>40</v>
@@ -2662,19 +2674,19 @@
         <v>52</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F49" s="8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G49" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H49" s="9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I49" s="10" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J49" s="11" t="s">
         <v>16</v>
@@ -2686,7 +2698,7 @@
         <v>48</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C50" s="8" t="s">
         <v>31</v>
@@ -2695,10 +2707,10 @@
         <v>52</v>
       </c>
       <c r="E50" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="F50" s="8" t="s">
         <v>120</v>
-      </c>
-      <c r="F50" s="8" t="s">
-        <v>122</v>
       </c>
       <c r="G50" s="8" t="s">
         <v>13</v>
@@ -2716,7 +2728,7 @@
         <v>49</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C51" s="8" t="s">
         <v>63</v>
@@ -2725,22 +2737,22 @@
         <v>65</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F51" s="8" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G51" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H51" s="9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I51" s="10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="J51" s="10" t="s">
-        <v>66</v>
+        <v>170</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2749,7 +2761,7 @@
         <v>50</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C52" s="8" t="s">
         <v>64</v>
@@ -2758,22 +2770,22 @@
         <v>65</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F52" s="8" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G52" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H52" s="9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I52" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="J52" s="10" t="s">
-        <v>67</v>
+        <v>171</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2782,7 +2794,7 @@
         <v>51</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C53" s="8" t="s">
         <v>40</v>
@@ -2791,10 +2803,10 @@
         <v>22</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F53" s="8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G53" s="8" t="s">
         <v>13</v>
@@ -2812,7 +2824,7 @@
         <v>52</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C54" s="8" t="s">
         <v>63</v>
@@ -2821,10 +2833,10 @@
         <v>65</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F54" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G54" s="8" t="s">
         <v>13</v>
@@ -2833,7 +2845,7 @@
         <v>10</v>
       </c>
       <c r="J54" s="10" t="s">
-        <v>66</v>
+        <v>170</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2842,7 +2854,7 @@
         <v>53</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C55" s="8" t="s">
         <v>64</v>
@@ -2851,10 +2863,10 @@
         <v>65</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F55" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G55" s="8" t="s">
         <v>13</v>
@@ -2863,7 +2875,7 @@
         <v>10</v>
       </c>
       <c r="J55" s="10" t="s">
-        <v>67</v>
+        <v>171</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
@@ -2872,28 +2884,28 @@
         <v>54</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C56" s="8" t="s">
         <v>40</v>
       </c>
       <c r="D56" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E56" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="F56" s="8" t="s">
         <v>145</v>
-      </c>
-      <c r="E56" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="F56" s="8" t="s">
-        <v>147</v>
       </c>
       <c r="G56" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H56" s="9" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="I56" s="10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="J56" s="11" t="s">
         <v>16</v>
@@ -2905,19 +2917,19 @@
         <v>55</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C57" s="8" t="s">
         <v>32</v>
       </c>
       <c r="D57" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E57" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="F57" s="8" t="s">
         <v>145</v>
-      </c>
-      <c r="E57" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="F57" s="8" t="s">
-        <v>147</v>
       </c>
       <c r="G57" s="8" t="s">
         <v>13</v>
@@ -2926,10 +2938,10 @@
         <v>43</v>
       </c>
       <c r="I57" s="10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J57" s="10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
@@ -2938,25 +2950,25 @@
         <v>56</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C58" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E58" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="D58" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="E58" s="7" t="s">
-        <v>146</v>
-      </c>
       <c r="F58" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G58" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H58" s="9" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="I58" s="10" t="s">
         <v>10</v>
@@ -2971,19 +2983,19 @@
         <v>57</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C59" s="8" t="s">
         <v>32</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F59" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G59" s="8" t="s">
         <v>13</v>
@@ -2992,10 +3004,10 @@
         <v>43</v>
       </c>
       <c r="I59" s="10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J59" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3004,19 +3016,19 @@
         <v>58</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C60" s="8" t="s">
         <v>32</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F60" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G60" s="8" t="s">
         <v>13</v>
@@ -3025,10 +3037,10 @@
         <v>43</v>
       </c>
       <c r="I60" s="10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J60" s="10" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3037,19 +3049,19 @@
         <v>59</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F61" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G61" s="8" t="s">
         <v>13</v>
@@ -3058,22 +3070,70 @@
         <v>43</v>
       </c>
       <c r="I61" s="10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J61" s="10" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="8">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B62" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E62" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F62" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="G62" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I62" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J62" s="10" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="8">
         <f t="shared" si="0"/>
         <v>61</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C63" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E63" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F63" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="G63" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I63" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J63" s="10" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Regressietesten voor GCO-555 toegevoegd
</commit_message>
<xml_diff>
--- a/catalogusdata/Logische testen Catalogus.xlsx
+++ b/catalogusdata/Logische testen Catalogus.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="187">
   <si>
     <t>US</t>
   </si>
@@ -80,9 +80,6 @@
   </si>
   <si>
     <t>GCO-391</t>
-  </si>
-  <si>
-    <t>Container geeft als foutmelding "De upload mag geen concepten of collecties zonder term bevatten."</t>
   </si>
   <si>
     <t>GCO-4</t>
@@ -606,6 +603,59 @@
   </si>
   <si>
     <t>Container geeft als foutmelding "De upload mag geen concepten of collecties zonder of met leeg skos:prefLabel bevatten."</t>
+  </si>
+  <si>
+    <t>Container geeft als foutmelding "De upload mag geen concepten of collecties zonder of met lege term bevatten."</t>
+  </si>
+  <si>
+    <t>Validatie lege term</t>
+  </si>
+  <si>
+    <t>Omgevingsdocumenten/Regressietest/Validatie lege term.xml</t>
+  </si>
+  <si>
+    <t>Omgevingsdocumenten/Regressietest/Datacontrole attributen.xml
+Omgevingsdocumenten/Regressietest/Validatie lege term.xml</t>
+  </si>
+  <si>
+    <t>Testbestand "Validatie lege term.xml" wordt geupload</t>
+  </si>
+  <si>
+    <t>GCO-555</t>
+  </si>
+  <si>
+    <t>Concepten/Regressietest/ttl/Datacontrole attributen.ttl
+Concepten/Regressietest/ttl/Validatie leeg label.ttl</t>
+  </si>
+  <si>
+    <t>Concepten/Regressietest/ttl/Datacontrole attributen.ttl
+Concepten/Regressietest/ttl/Validatie leeg prefLabel.ttl</t>
+  </si>
+  <si>
+    <t>Testbestand "Validatie leeg label.ttl" wordt geupload</t>
+  </si>
+  <si>
+    <t>Testbestand "Validatie leeg prefLabel.ttl" wordt geupload</t>
+  </si>
+  <si>
+    <t>Concepten/Regressietest/jsonld/Validatie leeg label.jsonld</t>
+  </si>
+  <si>
+    <t>Concepten/Regressietest/jsonld/Validatie leeg prefLabel.jsonld</t>
+  </si>
+  <si>
+    <t>Concepten/Regressietest/jsonld/Datacontrole attributen.jsonld
+Concepten/Regressietest/jsonld/Validatie leeg label.jsonld</t>
+  </si>
+  <si>
+    <t>Concepten/Regressietest/jsonld/Datacontrole attributen.jsonld
+Concepten/Regressietest/jsonld/Validatie leeg prefLabel.jsonld</t>
+  </si>
+  <si>
+    <t>Testbestand "Validatie leeg label.jsonld" wordt geupload</t>
+  </si>
+  <si>
+    <t>Testbestand "Validatie leeg prefLabel.jsonld" wordt geupload</t>
   </si>
 </sst>
 </file>
@@ -1126,10 +1176,10 @@
   <dimension ref="A1:J1376"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="D69" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J5" sqref="J5"/>
+      <selection pane="bottomRight" activeCell="I74" sqref="I74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1147,7 +1197,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -1170,10 +1220,10 @@
         <v>9</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>0</v>
@@ -1198,10 +1248,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>7</v>
@@ -1210,7 +1260,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>13</v>
@@ -1228,10 +1278,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>7</v>
@@ -1240,13 +1290,13 @@
         <v>6</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I4" s="10" t="s">
         <v>14</v>
@@ -1261,10 +1311,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>39</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>40</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>7</v>
@@ -1273,16 +1323,16 @@
         <v>11</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J5" s="11" t="s">
         <v>16</v>
@@ -1294,10 +1344,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>7</v>
@@ -1306,7 +1356,7 @@
         <v>11</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>13</v>
@@ -1324,10 +1374,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>18</v>
@@ -1336,19 +1386,19 @@
         <v>6</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>19</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I7" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="159" customHeight="1" x14ac:dyDescent="0.25">
@@ -1357,10 +1407,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>20</v>
@@ -1369,19 +1419,19 @@
         <v>6</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>19</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -1390,10 +1440,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>18</v>
@@ -1402,31 +1452,31 @@
         <v>11</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>19</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I9" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>18</v>
@@ -1435,7 +1485,7 @@
         <v>6</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>13</v>
@@ -1444,7 +1494,7 @@
         <v>10</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>21</v>
+        <v>171</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -1453,10 +1503,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>18</v>
@@ -1465,19 +1515,19 @@
         <v>11</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G11" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I11" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>21</v>
+        <v>171</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1486,19 +1536,19 @@
         <v>10</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="7" t="s">
-        <v>23</v>
-      </c>
       <c r="F12" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>13</v>
@@ -1516,19 +1566,19 @@
         <v>11</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G13" s="8" t="s">
         <v>13</v>
@@ -1537,7 +1587,7 @@
         <v>10</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1546,19 +1596,19 @@
         <v>12</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C14" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="E14" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G14" s="8" t="s">
         <v>13</v>
@@ -1567,40 +1617,40 @@
         <v>10</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="225" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B15" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>92</v>
-      </c>
       <c r="F15" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G15" s="8" t="s">
         <v>19</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -1609,31 +1659,31 @@
         <v>14</v>
       </c>
       <c r="B16" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>92</v>
-      </c>
       <c r="F16" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G16" s="8" t="s">
         <v>19</v>
       </c>
       <c r="H16" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="J16" s="10" t="s">
         <v>86</v>
-      </c>
-      <c r="I16" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="J16" s="10" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="273" customHeight="1" x14ac:dyDescent="0.25">
@@ -1642,31 +1692,31 @@
         <v>15</v>
       </c>
       <c r="B17" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C17" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>92</v>
-      </c>
       <c r="F17" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G17" s="8" t="s">
         <v>19</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I17" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -1675,31 +1725,31 @@
         <v>16</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G18" s="8" t="s">
         <v>19</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I18" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -1708,31 +1758,31 @@
         <v>17</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G19" s="8" t="s">
         <v>19</v>
       </c>
       <c r="H19" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I19" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1741,31 +1791,31 @@
         <v>18</v>
       </c>
       <c r="B20" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C20" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>92</v>
-      </c>
       <c r="F20" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G20" s="8" t="s">
         <v>19</v>
       </c>
       <c r="H20" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I20" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -1774,31 +1824,31 @@
         <v>19</v>
       </c>
       <c r="B21" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C21" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>92</v>
-      </c>
       <c r="F21" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G21" s="8" t="s">
         <v>19</v>
       </c>
       <c r="H21" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I21" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="J21" s="10" t="s">
         <v>93</v>
-      </c>
-      <c r="J21" s="10" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1807,31 +1857,31 @@
         <v>20</v>
       </c>
       <c r="B22" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="F22" s="8" t="s">
         <v>111</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>112</v>
       </c>
       <c r="G22" s="8" t="s">
         <v>19</v>
       </c>
       <c r="H22" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J22" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -1840,31 +1890,31 @@
         <v>21</v>
       </c>
       <c r="B23" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C23" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>92</v>
-      </c>
       <c r="F23" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G23" s="8" t="s">
         <v>19</v>
       </c>
       <c r="H23" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I23" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J23" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -1873,31 +1923,31 @@
         <v>22</v>
       </c>
       <c r="B24" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C24" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>92</v>
-      </c>
       <c r="F24" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G24" s="8" t="s">
         <v>19</v>
       </c>
       <c r="H24" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I24" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J24" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -1906,31 +1956,31 @@
         <v>23</v>
       </c>
       <c r="B25" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C25" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>92</v>
-      </c>
       <c r="F25" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G25" s="8" t="s">
         <v>19</v>
       </c>
       <c r="H25" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I25" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J25" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -1939,31 +1989,31 @@
         <v>24</v>
       </c>
       <c r="B26" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C26" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>92</v>
-      </c>
       <c r="F26" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G26" s="8" t="s">
         <v>19</v>
       </c>
       <c r="H26" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I26" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J26" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1972,31 +2022,31 @@
         <v>25</v>
       </c>
       <c r="B27" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E27" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C27" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>92</v>
-      </c>
       <c r="F27" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G27" s="8" t="s">
         <v>19</v>
       </c>
       <c r="H27" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I27" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="J27" s="10" t="s">
         <v>98</v>
-      </c>
-      <c r="J27" s="10" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2005,31 +2055,31 @@
         <v>26</v>
       </c>
       <c r="B28" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C28" s="8" t="s">
-        <v>37</v>
-      </c>
       <c r="D28" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G28" s="8" t="s">
         <v>19</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I28" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="J28" s="10" t="s">
         <v>26</v>
-      </c>
-      <c r="J28" s="10" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2038,19 +2088,19 @@
         <v>27</v>
       </c>
       <c r="B29" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C29" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="E29" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G29" s="8" t="s">
         <v>13</v>
@@ -2068,25 +2118,25 @@
         <v>28</v>
       </c>
       <c r="B30" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C30" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="E30" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G30" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H30" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I30" s="10" t="s">
         <v>14</v>
@@ -2101,19 +2151,19 @@
         <v>29</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G31" s="8" t="s">
         <v>13</v>
@@ -2122,7 +2172,7 @@
         <v>10</v>
       </c>
       <c r="J31" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2131,19 +2181,19 @@
         <v>30</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C32" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="E32" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G32" s="8" t="s">
         <v>13</v>
@@ -2152,7 +2202,7 @@
         <v>10</v>
       </c>
       <c r="J32" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2161,28 +2211,28 @@
         <v>31</v>
       </c>
       <c r="B33" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E33" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C33" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>57</v>
-      </c>
       <c r="F33" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G33" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H33" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I33" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J33" s="11" t="s">
         <v>16</v>
@@ -2194,19 +2244,19 @@
         <v>32</v>
       </c>
       <c r="B34" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E34" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C34" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>57</v>
-      </c>
       <c r="F34" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>13</v>
@@ -2224,31 +2274,31 @@
         <v>33</v>
       </c>
       <c r="B35" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E35" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C35" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>57</v>
-      </c>
       <c r="F35" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G35" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H35" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I35" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J35" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2257,31 +2307,31 @@
         <v>34</v>
       </c>
       <c r="B36" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E36" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C36" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>57</v>
-      </c>
       <c r="F36" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G36" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H36" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I36" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J36" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2290,19 +2340,19 @@
         <v>35</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E37" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="F37" s="8" t="s">
         <v>78</v>
-      </c>
-      <c r="F37" s="8" t="s">
-        <v>79</v>
       </c>
       <c r="G37" s="8" t="s">
         <v>13</v>
@@ -2320,25 +2370,25 @@
         <v>36</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E38" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="F38" s="8" t="s">
         <v>78</v>
-      </c>
-      <c r="F38" s="8" t="s">
-        <v>79</v>
       </c>
       <c r="G38" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H38" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I38" s="10" t="s">
         <v>14</v>
@@ -2353,19 +2403,19 @@
         <v>37</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G39" s="8" t="s">
         <v>13</v>
@@ -2374,7 +2424,7 @@
         <v>10</v>
       </c>
       <c r="J39" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2383,19 +2433,19 @@
         <v>38</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C40" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D40" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="E40" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G40" s="8" t="s">
         <v>13</v>
@@ -2404,7 +2454,7 @@
         <v>10</v>
       </c>
       <c r="J40" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2413,28 +2463,28 @@
         <v>39</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G41" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H41" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I41" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J41" s="11" t="s">
         <v>16</v>
@@ -2446,19 +2496,19 @@
         <v>40</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G42" s="8" t="s">
         <v>13</v>
@@ -2476,31 +2526,31 @@
         <v>41</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G43" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H43" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I43" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J43" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2509,31 +2559,31 @@
         <v>42</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C44" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D44" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D44" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="E44" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G44" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H44" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I44" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J44" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2542,19 +2592,19 @@
         <v>43</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G45" s="8" t="s">
         <v>13</v>
@@ -2572,25 +2622,25 @@
         <v>44</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F46" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G46" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H46" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I46" s="10" t="s">
         <v>14</v>
@@ -2605,19 +2655,19 @@
         <v>45</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G47" s="8" t="s">
         <v>13</v>
@@ -2626,7 +2676,7 @@
         <v>10</v>
       </c>
       <c r="J47" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2635,19 +2685,19 @@
         <v>46</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C48" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D48" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D48" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="E48" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F48" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G48" s="8" t="s">
         <v>13</v>
@@ -2656,7 +2706,7 @@
         <v>10</v>
       </c>
       <c r="J48" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2665,28 +2715,28 @@
         <v>47</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F49" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G49" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H49" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I49" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J49" s="11" t="s">
         <v>16</v>
@@ -2698,19 +2748,19 @@
         <v>48</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F50" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G50" s="8" t="s">
         <v>13</v>
@@ -2728,31 +2778,31 @@
         <v>49</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F51" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G51" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H51" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I51" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J51" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2761,31 +2811,31 @@
         <v>50</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C52" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D52" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D52" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="E52" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F52" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G52" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H52" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I52" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J52" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2794,19 +2844,19 @@
         <v>51</v>
       </c>
       <c r="B53" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E53" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="C53" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E53" s="7" t="s">
-        <v>124</v>
-      </c>
       <c r="F53" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G53" s="8" t="s">
         <v>13</v>
@@ -2824,19 +2874,19 @@
         <v>52</v>
       </c>
       <c r="B54" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E54" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="C54" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E54" s="7" t="s">
-        <v>124</v>
-      </c>
       <c r="F54" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G54" s="8" t="s">
         <v>13</v>
@@ -2845,7 +2895,7 @@
         <v>10</v>
       </c>
       <c r="J54" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2854,19 +2904,19 @@
         <v>53</v>
       </c>
       <c r="B55" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E55" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="C55" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E55" s="7" t="s">
-        <v>124</v>
-      </c>
       <c r="F55" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G55" s="8" t="s">
         <v>13</v>
@@ -2875,7 +2925,7 @@
         <v>10</v>
       </c>
       <c r="J55" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
@@ -2884,28 +2934,28 @@
         <v>54</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D56" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E56" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="E56" s="7" t="s">
+      <c r="F56" s="8" t="s">
         <v>144</v>
-      </c>
-      <c r="F56" s="8" t="s">
-        <v>145</v>
       </c>
       <c r="G56" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H56" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="I56" s="10" t="s">
         <v>146</v>
-      </c>
-      <c r="I56" s="10" t="s">
-        <v>147</v>
       </c>
       <c r="J56" s="11" t="s">
         <v>16</v>
@@ -2917,31 +2967,31 @@
         <v>55</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F57" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G57" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H57" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I57" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J57" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
@@ -2950,25 +3000,25 @@
         <v>56</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D58" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E58" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="F58" s="8" t="s">
         <v>149</v>
-      </c>
-      <c r="E58" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="F58" s="8" t="s">
-        <v>150</v>
       </c>
       <c r="G58" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H58" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I58" s="10" t="s">
         <v>10</v>
@@ -2983,31 +3033,31 @@
         <v>57</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D59" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E59" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="F59" s="8" t="s">
         <v>149</v>
-      </c>
-      <c r="E59" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="F59" s="8" t="s">
-        <v>150</v>
       </c>
       <c r="G59" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H59" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I59" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J59" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3016,31 +3066,31 @@
         <v>58</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D60" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E60" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="F60" s="8" t="s">
         <v>149</v>
-      </c>
-      <c r="E60" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="F60" s="8" t="s">
-        <v>150</v>
       </c>
       <c r="G60" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H60" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I60" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J60" s="10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3049,31 +3099,31 @@
         <v>59</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C61" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E61" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="F61" s="8" t="s">
         <v>152</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E61" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="F61" s="8" t="s">
-        <v>153</v>
       </c>
       <c r="G61" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H61" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I61" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J61" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3082,19 +3132,19 @@
         <v>60</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>65</v>
+        <v>176</v>
       </c>
       <c r="E62" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F62" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G62" s="8" t="s">
         <v>13</v>
@@ -3103,7 +3153,7 @@
         <v>10</v>
       </c>
       <c r="J62" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3112,19 +3162,19 @@
         <v>61</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>65</v>
+        <v>176</v>
       </c>
       <c r="E63" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F63" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G63" s="8" t="s">
         <v>13</v>
@@ -3133,106 +3183,361 @@
         <v>10</v>
       </c>
       <c r="J63" s="10" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="8">
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B64" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C64" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E64" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F64" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="G64" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I64" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J64" s="10" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A65" s="8">
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B65" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C65" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E65" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F65" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="G65" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H65" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I65" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="J65" s="10" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="8">
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B66" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C66" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E66" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F66" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="G66" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I66" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J66" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="8">
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B67" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C67" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E67" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F67" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="G67" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I67" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J67" s="10" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A68" s="8">
         <f t="shared" si="0"/>
         <v>66</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B68" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C68" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E68" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F68" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="G68" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H68" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="I68" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="J68" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A69" s="8">
         <f t="shared" ref="A69:A132" si="1">A68+1</f>
         <v>67</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B69" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C69" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E69" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F69" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="G69" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H69" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="I69" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="J69" s="10" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="8">
         <f t="shared" si="1"/>
         <v>68</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B70" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C70" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E70" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="F70" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="G70" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I70" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J70" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="8">
         <f t="shared" si="1"/>
         <v>69</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B71" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C71" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E71" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="F71" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="G71" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I71" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J71" s="10" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A72" s="8">
         <f t="shared" si="1"/>
         <v>70</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B72" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C72" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E72" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="F72" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="G72" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H72" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="I72" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="J72" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A73" s="8">
         <f t="shared" si="1"/>
         <v>71</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B73" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C73" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E73" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="F73" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="G73" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H73" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="I73" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="J73" s="10" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="8">
         <f t="shared" si="1"/>
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="8">
         <f t="shared" si="1"/>
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="8">
         <f t="shared" si="1"/>
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="8">
         <f t="shared" si="1"/>
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="8">
         <f t="shared" si="1"/>
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="8">
         <f t="shared" si="1"/>
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="8">
         <f t="shared" si="1"/>
         <v>78</v>

</xml_diff>

<commit_message>
Regressietesten toegevoegd voor GCO-53
</commit_message>
<xml_diff>
--- a/catalogusdata/Logische testen Catalogus.xlsx
+++ b/catalogusdata/Logische testen Catalogus.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="194">
   <si>
     <t>US</t>
   </si>
@@ -40,9 +40,6 @@
     <t>container/concepten-post-xml</t>
   </si>
   <si>
-    <t>GCO-450</t>
-  </si>
-  <si>
     <t>Testbestand(en)</t>
   </si>
   <si>
@@ -73,25 +70,13 @@
     <t>Container geeft als foutmelding "De upload bevat concepten die nog niet bestaan"</t>
   </si>
   <si>
-    <t>GCO-382</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
-    <t>GCO-391</t>
-  </si>
-  <si>
-    <t>GCO-4</t>
-  </si>
-  <si>
     <t>container/ttlupdate</t>
   </si>
   <si>
     <t>Pagina /id/concept/GeneriekBeest wordt bekeken</t>
-  </si>
-  <si>
-    <t>GCO-294</t>
   </si>
   <si>
     <t>Pagina /query/search?term=monster wordt bekeken</t>
@@ -177,9 +162,6 @@
     <t>Concepten POST Turtle</t>
   </si>
   <si>
-    <t>GCO-470</t>
-  </si>
-  <si>
     <t>query/search</t>
   </si>
   <si>
@@ -215,9 +197,6 @@
   </si>
   <si>
     <t>Validatie prefLabel</t>
-  </si>
-  <si>
-    <t>GCO-466</t>
   </si>
   <si>
     <t>Testbestand "Datacontrole attributen.xml" is geupload via /container/concepten-post-xml</t>
@@ -506,9 +485,6 @@
     <t>Upload controle</t>
   </si>
   <si>
-    <t>GCO-540</t>
-  </si>
-  <si>
     <t>container/datasetupload</t>
   </si>
   <si>
@@ -528,9 +504,6 @@
 - Beschrijving | Een Catalogus voor Testdoeleinden</t>
   </si>
   <si>
-    <t>GCO-526</t>
-  </si>
-  <si>
     <t>Dataset T.ttl</t>
   </si>
   <si>
@@ -621,9 +594,6 @@
     <t>Testbestand "Validatie lege term.xml" wordt geupload</t>
   </si>
   <si>
-    <t>GCO-555</t>
-  </si>
-  <si>
     <t>Concepten/Regressietest/ttl/Datacontrole attributen.ttl
 Concepten/Regressietest/ttl/Validatie leeg label.ttl</t>
   </si>
@@ -656,6 +626,60 @@
   </si>
   <si>
     <t>Testbestand "Validatie leeg prefLabel.jsonld" wordt geupload</t>
+  </si>
+  <si>
+    <t>Weergavepagina Toeleidingsbegrippen</t>
+  </si>
+  <si>
+    <t>Datacontrole</t>
+  </si>
+  <si>
+    <t>O - GCO-450</t>
+  </si>
+  <si>
+    <t>O - GCO-382</t>
+  </si>
+  <si>
+    <t>O - GCO-391</t>
+  </si>
+  <si>
+    <t>O - GCO-4</t>
+  </si>
+  <si>
+    <t>O - GCO-466</t>
+  </si>
+  <si>
+    <t>O - GCO-294</t>
+  </si>
+  <si>
+    <t>O - GCO-470</t>
+  </si>
+  <si>
+    <t>O - GCO-540</t>
+  </si>
+  <si>
+    <t>O - GCO-526</t>
+  </si>
+  <si>
+    <t>O - GCO-555</t>
+  </si>
+  <si>
+    <t>GCO-53</t>
+  </si>
+  <si>
+    <t>query/toeleidingsbegrippen</t>
+  </si>
+  <si>
+    <t>Op de pagina staat o.a. een tabel met:
+- als headers 'Toeleidingsbegrip' en 'Concept'
+- één rij met in de eerste kolom 'monster' en in de tweede kolom een link naar /id/concept/GeneriekBeest met als label 'Generiek beest'</t>
+  </si>
+  <si>
+    <t>Op de volgende link geklikt wordt:
+- id/concept/GeneriekBeest</t>
+  </si>
+  <si>
+    <t>De weergavepagina voor GeneriekBeest wordt geopend in hetzelfde scherm.</t>
   </si>
 </sst>
 </file>
@@ -1176,10 +1200,10 @@
   <dimension ref="A1:J1376"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="D69" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B70" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I74" sqref="I74"/>
+      <selection pane="bottomRight" activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1197,7 +1221,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -1217,13 +1241,13 @@
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>0</v>
@@ -1232,10 +1256,10 @@
         <v>4</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>5</v>
@@ -1248,28 +1272,28 @@
         <v>1</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>7</v>
+        <v>179</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>6</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J3" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1278,31 +1302,31 @@
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>7</v>
+        <v>179</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>6</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="I4" s="10" t="s">
+      <c r="J4" s="10" t="s">
         <v>14</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -1311,31 +1335,31 @@
         <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="I5" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>43</v>
-      </c>
       <c r="J5" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1344,28 +1368,28 @@
         <v>4</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>7</v>
+        <v>179</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="135" x14ac:dyDescent="0.25">
@@ -1374,31 +1398,31 @@
         <v>5</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>18</v>
+        <v>180</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>6</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="G7" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="I7" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="I7" s="10" t="s">
-        <v>23</v>
-      </c>
       <c r="J7" s="10" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="159" customHeight="1" x14ac:dyDescent="0.25">
@@ -1407,31 +1431,31 @@
         <v>6</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>20</v>
+        <v>181</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H8" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="I8" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="I8" s="10" t="s">
-        <v>47</v>
-      </c>
       <c r="J8" s="10" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -1440,31 +1464,31 @@
         <v>7</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C9" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>45</v>
-      </c>
       <c r="G9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="I9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="I9" s="10" t="s">
-        <v>23</v>
-      </c>
       <c r="J9" s="10" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1473,28 +1497,28 @@
         <v>8</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>18</v>
+        <v>180</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>6</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -1503,31 +1527,31 @@
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>18</v>
+        <v>180</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="I11" s="10" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1536,28 +1560,28 @@
         <v>10</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>21</v>
+        <v>182</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1566,28 +1590,28 @@
         <v>11</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>64</v>
+        <v>183</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I13" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1596,28 +1620,28 @@
         <v>12</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>64</v>
+        <v>183</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="165" x14ac:dyDescent="0.25">
@@ -1626,31 +1650,31 @@
         <v>13</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>21</v>
+        <v>182</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -1659,31 +1683,31 @@
         <v>14</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>21</v>
+        <v>182</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H16" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="I16" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="I16" s="10" t="s">
-        <v>92</v>
-      </c>
       <c r="J16" s="10" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="273" customHeight="1" x14ac:dyDescent="0.25">
@@ -1692,31 +1716,31 @@
         <v>15</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>21</v>
+        <v>182</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="I17" s="10" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -1725,31 +1749,31 @@
         <v>16</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>21</v>
+        <v>182</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="I18" s="10" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -1758,31 +1782,31 @@
         <v>17</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>21</v>
+        <v>182</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H19" s="9" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="I19" s="10" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1791,31 +1815,31 @@
         <v>18</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>24</v>
+        <v>184</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H20" s="9" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="I20" s="10" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -1824,31 +1848,31 @@
         <v>19</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>21</v>
+        <v>182</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H21" s="9" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="I21" s="10" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1857,31 +1881,31 @@
         <v>20</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>21</v>
+        <v>182</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H22" s="9" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="J22" s="10" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -1890,31 +1914,31 @@
         <v>21</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>21</v>
+        <v>182</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H23" s="9" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="I23" s="10" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="J23" s="10" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -1923,31 +1947,31 @@
         <v>22</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>21</v>
+        <v>182</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H24" s="9" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="I24" s="10" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="J24" s="10" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -1956,31 +1980,31 @@
         <v>23</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>24</v>
+        <v>184</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H25" s="9" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="I25" s="10" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="J25" s="10" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -1989,31 +2013,31 @@
         <v>24</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>21</v>
+        <v>182</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H26" s="9" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="I26" s="10" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="J26" s="10" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2022,31 +2046,31 @@
         <v>25</v>
       </c>
       <c r="B27" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H27" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="I27" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C27" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E27" s="7" t="s">
+      <c r="J27" s="10" t="s">
         <v>91</v>
-      </c>
-      <c r="F27" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="G27" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="H27" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="I27" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="J27" s="10" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2055,31 +2079,31 @@
         <v>26</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>24</v>
+        <v>184</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="I28" s="10" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="J28" s="10" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2088,28 +2112,28 @@
         <v>27</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>51</v>
+        <v>185</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I29" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J29" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2118,31 +2142,31 @@
         <v>28</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>51</v>
+        <v>185</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="G30" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H30" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="I30" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="H30" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="I30" s="10" t="s">
+      <c r="J30" s="10" t="s">
         <v>14</v>
-      </c>
-      <c r="J30" s="10" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2151,28 +2175,28 @@
         <v>29</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>64</v>
+        <v>183</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I31" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J31" s="10" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2181,28 +2205,28 @@
         <v>30</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>64</v>
+        <v>183</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I32" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J32" s="10" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2211,31 +2235,31 @@
         <v>31</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D33" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H33" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="I33" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="E33" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F33" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="G33" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H33" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="I33" s="10" t="s">
-        <v>57</v>
-      </c>
       <c r="J33" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2244,28 +2268,28 @@
         <v>32</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>51</v>
+        <v>185</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I34" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J34" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2274,31 +2298,31 @@
         <v>33</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>64</v>
+        <v>183</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="G35" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H35" s="9" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="I35" s="10" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="J35" s="10" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2307,31 +2331,31 @@
         <v>34</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>64</v>
+        <v>183</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H36" s="9" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="I36" s="10" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="J36" s="10" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2340,28 +2364,28 @@
         <v>35</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>51</v>
+        <v>185</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I37" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J37" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2370,31 +2394,31 @@
         <v>36</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>51</v>
+        <v>185</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="G38" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H38" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="I38" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="H38" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="I38" s="10" t="s">
+      <c r="J38" s="10" t="s">
         <v>14</v>
-      </c>
-      <c r="J38" s="10" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2403,28 +2427,28 @@
         <v>37</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>64</v>
+        <v>183</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I39" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J39" s="10" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2433,28 +2457,28 @@
         <v>38</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>64</v>
+        <v>183</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I40" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J40" s="10" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2463,31 +2487,31 @@
         <v>39</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>51</v>
+        <v>185</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="G41" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H41" s="9" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="I41" s="10" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="J41" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2496,28 +2520,28 @@
         <v>40</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>51</v>
+        <v>185</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I42" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J42" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2526,31 +2550,31 @@
         <v>41</v>
       </c>
       <c r="B43" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="G43" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H43" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="I43" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="C43" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E43" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="F43" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="G43" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H43" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="I43" s="10" t="s">
-        <v>83</v>
-      </c>
       <c r="J43" s="10" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2559,31 +2583,31 @@
         <v>42</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>64</v>
+        <v>183</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="G44" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H44" s="9" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="I44" s="10" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="J44" s="10" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2592,28 +2616,28 @@
         <v>43</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>51</v>
+        <v>185</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="G45" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I45" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J45" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2622,31 +2646,31 @@
         <v>44</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>51</v>
+        <v>185</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="F46" s="8" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="G46" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H46" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="I46" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="H46" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="I46" s="10" t="s">
+      <c r="J46" s="10" t="s">
         <v>14</v>
-      </c>
-      <c r="J46" s="10" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2655,28 +2679,28 @@
         <v>45</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>64</v>
+        <v>183</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="G47" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I47" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J47" s="10" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2685,28 +2709,28 @@
         <v>46</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>64</v>
+        <v>183</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="F48" s="8" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="G48" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I48" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J48" s="10" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2715,31 +2739,31 @@
         <v>47</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>51</v>
+        <v>185</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="F49" s="8" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="G49" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H49" s="9" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="I49" s="10" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="J49" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2748,28 +2772,28 @@
         <v>48</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>51</v>
+        <v>185</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="F50" s="8" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="G50" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I50" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J50" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2778,31 +2802,31 @@
         <v>49</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>64</v>
+        <v>183</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="F51" s="8" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="G51" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H51" s="9" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="I51" s="10" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="J51" s="10" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2811,31 +2835,31 @@
         <v>50</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>64</v>
+        <v>183</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="F52" s="8" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="G52" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H52" s="9" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="I52" s="10" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="J52" s="10" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2844,28 +2868,28 @@
         <v>51</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>21</v>
+        <v>182</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="F53" s="8" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="G53" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I53" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J53" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2874,28 +2898,28 @@
         <v>52</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>64</v>
+        <v>183</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="F54" s="8" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="G54" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I54" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J54" s="10" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2904,28 +2928,28 @@
         <v>53</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>64</v>
+        <v>183</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="F55" s="8" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="G55" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I55" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J55" s="10" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
@@ -2934,31 +2958,31 @@
         <v>54</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>142</v>
+        <v>186</v>
       </c>
       <c r="E56" s="7" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="F56" s="8" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="G56" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H56" s="9" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="I56" s="10" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="J56" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -2967,31 +2991,31 @@
         <v>55</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>142</v>
+        <v>186</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="F57" s="8" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="G57" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H57" s="9" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="I57" s="10" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="J57" s="10" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
@@ -3000,31 +3024,31 @@
         <v>56</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>148</v>
+        <v>187</v>
       </c>
       <c r="E58" s="7" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="F58" s="8" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="G58" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H58" s="9" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="I58" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J58" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3033,31 +3057,31 @@
         <v>57</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>148</v>
+        <v>187</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="F59" s="8" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="G59" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H59" s="9" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="I59" s="10" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="J59" s="10" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3066,31 +3090,31 @@
         <v>58</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>148</v>
+        <v>187</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="F60" s="8" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="G60" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H60" s="9" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="I60" s="10" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="J60" s="10" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3099,31 +3123,31 @@
         <v>59</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>148</v>
+        <v>187</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="F61" s="8" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="G61" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H61" s="9" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="I61" s="10" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="J61" s="10" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3132,28 +3156,28 @@
         <v>60</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>176</v>
+        <v>188</v>
       </c>
       <c r="E62" s="7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F62" s="8" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="G62" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I62" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J62" s="10" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3162,28 +3186,28 @@
         <v>61</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>176</v>
+        <v>188</v>
       </c>
       <c r="E63" s="7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F63" s="8" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="G63" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I63" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J63" s="10" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3192,28 +3216,28 @@
         <v>62</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>176</v>
+        <v>188</v>
       </c>
       <c r="E64" s="7" t="s">
         <v>6</v>
       </c>
       <c r="F64" s="8" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="G64" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I64" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J64" s="10" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -3222,31 +3246,31 @@
         <v>63</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>176</v>
+        <v>188</v>
       </c>
       <c r="E65" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F65" s="8" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="G65" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H65" s="9" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="I65" s="10" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="J65" s="10" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3255,28 +3279,28 @@
         <v>64</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>176</v>
+        <v>188</v>
       </c>
       <c r="E66" s="7" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="F66" s="8" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="G66" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I66" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J66" s="10" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3285,28 +3309,28 @@
         <v>65</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>176</v>
+        <v>188</v>
       </c>
       <c r="E67" s="7" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="F67" s="8" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="G67" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I67" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J67" s="10" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -3315,31 +3339,31 @@
         <v>66</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>176</v>
+        <v>188</v>
       </c>
       <c r="E68" s="7" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="F68" s="8" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="G68" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H68" s="9" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="I68" s="10" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="J68" s="10" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -3348,31 +3372,31 @@
         <v>67</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>176</v>
+        <v>188</v>
       </c>
       <c r="E69" s="7" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="F69" s="8" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="G69" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H69" s="9" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="I69" s="10" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="J69" s="10" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3381,28 +3405,28 @@
         <v>68</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>176</v>
+        <v>188</v>
       </c>
       <c r="E70" s="7" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="F70" s="8" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="G70" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I70" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J70" s="10" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="71" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -3411,28 +3435,28 @@
         <v>69</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>176</v>
+        <v>188</v>
       </c>
       <c r="E71" s="7" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="F71" s="8" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="G71" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I71" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J71" s="10" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -3441,31 +3465,31 @@
         <v>70</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>176</v>
+        <v>188</v>
       </c>
       <c r="E72" s="7" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="F72" s="8" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="G72" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H72" s="9" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="I72" s="10" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="J72" s="10" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="73" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -3474,43 +3498,97 @@
         <v>71</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="D73" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E73" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F73" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="G73" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H73" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="I73" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="E73" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="F73" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="G73" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H73" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="I73" s="10" t="s">
-        <v>186</v>
-      </c>
       <c r="J73" s="10" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A74" s="8">
         <f t="shared" si="1"/>
         <v>72</v>
       </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B74" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="C74" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E74" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="F74" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="G74" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H74" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="I74" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="J74" s="10" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="8">
         <f t="shared" si="1"/>
         <v>73</v>
+      </c>
+      <c r="B75" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="C75" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E75" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="F75" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="G75" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H75" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="I75" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="J75" s="10" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Aanpassinge voor validatie toeleidingsbegrippen gedaan. Testbestanden gemaakt, en test procedure beschreven Tevens kleine aanpassing voor het tonen van afbeeldingen bij begrippen foaf:depiction gedaan
</commit_message>
<xml_diff>
--- a/catalogusdata/Logische testen Catalogus.xlsx
+++ b/catalogusdata/Logische testen Catalogus.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="212">
   <si>
     <t>US</t>
   </si>
@@ -722,6 +722,18 @@
   </si>
   <si>
     <t>Op de pagina staat o.a. een tabel met als header Dier en onder de waarde domein is TestSchema terug te zien</t>
+  </si>
+  <si>
+    <t>GCO-135</t>
+  </si>
+  <si>
+    <t>Validatie toeleidingsbegrippen</t>
+  </si>
+  <si>
+    <t>Concepten/Regeressietest/ttl/Validatie toeleidingsbegrip.ttl</t>
+  </si>
+  <si>
+    <t>Container geeft als resultaat "Toeleidingsbegrippen mogen enkel concepten met een rdfs:label, skos:prefLabel of skos:closeMatch bevatten."</t>
   </si>
 </sst>
 </file>
@@ -1239,13 +1251,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1376"/>
+  <dimension ref="A1:J1375"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="D72" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="D78" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G80" sqref="G80"/>
+      <selection pane="bottomRight" activeCell="J88" sqref="J88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3410,7 +3422,7 @@
     </row>
     <row r="69" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A69" s="8">
-        <f t="shared" ref="A69:A132" si="1">A68+1</f>
+        <f t="shared" ref="A69:A131" si="1">A68+1</f>
         <v>67</v>
       </c>
       <c r="B69" s="8" t="s">
@@ -3759,103 +3771,153 @@
         <v>207</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="8">
         <f t="shared" si="1"/>
         <v>78</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B80" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="C80" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E80" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F80" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="G80" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I80" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="J80" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" s="8">
-        <f t="shared" si="1"/>
         <v>79</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B81" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="C81" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E81" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F81" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="G81" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H81" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="I81" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="J81" s="10" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="8">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="8">
         <f t="shared" si="1"/>
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="8">
         <f t="shared" si="1"/>
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="8">
         <f t="shared" si="1"/>
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="8">
         <f t="shared" si="1"/>
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="8">
         <f t="shared" si="1"/>
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="8">
         <f t="shared" si="1"/>
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="8">
         <f t="shared" si="1"/>
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="8">
         <f t="shared" si="1"/>
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="8">
         <f t="shared" si="1"/>
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="8">
         <f t="shared" si="1"/>
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="8">
         <f t="shared" si="1"/>
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="8">
         <f t="shared" si="1"/>
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="8">
         <f t="shared" si="1"/>
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="8">
         <f t="shared" si="1"/>
         <v>94</v>
@@ -4073,13 +4135,13 @@
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="A132:A195" si="2">A131+1</f>
         <v>130</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" s="8">
-        <f t="shared" ref="A133:A196" si="2">A132+1</f>
+        <f t="shared" si="2"/>
         <v>131</v>
       </c>
     </row>
@@ -4457,13 +4519,13 @@
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A196" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="A196:A259" si="3">A195+1</f>
         <v>194</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A197" s="8">
-        <f t="shared" ref="A197:A260" si="3">A196+1</f>
+        <f t="shared" si="3"/>
         <v>195</v>
       </c>
     </row>
@@ -4841,13 +4903,13 @@
     </row>
     <row r="260" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A260" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="A260:A323" si="4">A259+1</f>
         <v>258</v>
       </c>
     </row>
     <row r="261" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A261" s="8">
-        <f t="shared" ref="A261:A324" si="4">A260+1</f>
+        <f t="shared" si="4"/>
         <v>259</v>
       </c>
     </row>
@@ -5225,13 +5287,13 @@
     </row>
     <row r="324" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A324" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="A324:A387" si="5">A323+1</f>
         <v>322</v>
       </c>
     </row>
     <row r="325" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A325" s="8">
-        <f t="shared" ref="A325:A388" si="5">A324+1</f>
+        <f t="shared" si="5"/>
         <v>323</v>
       </c>
     </row>
@@ -5609,13 +5671,13 @@
     </row>
     <row r="388" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A388" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="A388:A451" si="6">A387+1</f>
         <v>386</v>
       </c>
     </row>
     <row r="389" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A389" s="8">
-        <f t="shared" ref="A389:A452" si="6">A388+1</f>
+        <f t="shared" si="6"/>
         <v>387</v>
       </c>
     </row>
@@ -5993,13 +6055,13 @@
     </row>
     <row r="452" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A452" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="A452:A515" si="7">A451+1</f>
         <v>450</v>
       </c>
     </row>
     <row r="453" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A453" s="8">
-        <f t="shared" ref="A453:A516" si="7">A452+1</f>
+        <f t="shared" si="7"/>
         <v>451</v>
       </c>
     </row>
@@ -6377,13 +6439,13 @@
     </row>
     <row r="516" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A516" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="A516:A579" si="8">A515+1</f>
         <v>514</v>
       </c>
     </row>
     <row r="517" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A517" s="8">
-        <f t="shared" ref="A517:A580" si="8">A516+1</f>
+        <f t="shared" si="8"/>
         <v>515</v>
       </c>
     </row>
@@ -6761,13 +6823,13 @@
     </row>
     <row r="580" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A580" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="A580:A643" si="9">A579+1</f>
         <v>578</v>
       </c>
     </row>
     <row r="581" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A581" s="8">
-        <f t="shared" ref="A581:A644" si="9">A580+1</f>
+        <f t="shared" si="9"/>
         <v>579</v>
       </c>
     </row>
@@ -7145,13 +7207,13 @@
     </row>
     <row r="644" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A644" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="A644:A707" si="10">A643+1</f>
         <v>642</v>
       </c>
     </row>
     <row r="645" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A645" s="8">
-        <f t="shared" ref="A645:A708" si="10">A644+1</f>
+        <f t="shared" si="10"/>
         <v>643</v>
       </c>
     </row>
@@ -7529,13 +7591,13 @@
     </row>
     <row r="708" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A708" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="A708:A771" si="11">A707+1</f>
         <v>706</v>
       </c>
     </row>
     <row r="709" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A709" s="8">
-        <f t="shared" ref="A709:A772" si="11">A708+1</f>
+        <f t="shared" si="11"/>
         <v>707</v>
       </c>
     </row>
@@ -7913,13 +7975,13 @@
     </row>
     <row r="772" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A772" s="8">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="A772:A835" si="12">A771+1</f>
         <v>770</v>
       </c>
     </row>
     <row r="773" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A773" s="8">
-        <f t="shared" ref="A773:A836" si="12">A772+1</f>
+        <f t="shared" si="12"/>
         <v>771</v>
       </c>
     </row>
@@ -8297,13 +8359,13 @@
     </row>
     <row r="836" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A836" s="8">
-        <f t="shared" si="12"/>
+        <f t="shared" ref="A836:A899" si="13">A835+1</f>
         <v>834</v>
       </c>
     </row>
     <row r="837" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A837" s="8">
-        <f t="shared" ref="A837:A900" si="13">A836+1</f>
+        <f t="shared" si="13"/>
         <v>835</v>
       </c>
     </row>
@@ -8681,13 +8743,13 @@
     </row>
     <row r="900" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A900" s="8">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="A900:A963" si="14">A899+1</f>
         <v>898</v>
       </c>
     </row>
     <row r="901" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A901" s="8">
-        <f t="shared" ref="A901:A964" si="14">A900+1</f>
+        <f t="shared" si="14"/>
         <v>899</v>
       </c>
     </row>
@@ -9065,13 +9127,13 @@
     </row>
     <row r="964" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A964" s="8">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="A964:A1027" si="15">A963+1</f>
         <v>962</v>
       </c>
     </row>
     <row r="965" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A965" s="8">
-        <f t="shared" ref="A965:A1028" si="15">A964+1</f>
+        <f t="shared" si="15"/>
         <v>963</v>
       </c>
     </row>
@@ -9449,13 +9511,13 @@
     </row>
     <row r="1028" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1028" s="8">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="A1028:A1091" si="16">A1027+1</f>
         <v>1026</v>
       </c>
     </row>
     <row r="1029" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1029" s="8">
-        <f t="shared" ref="A1029:A1092" si="16">A1028+1</f>
+        <f t="shared" si="16"/>
         <v>1027</v>
       </c>
     </row>
@@ -9833,13 +9895,13 @@
     </row>
     <row r="1092" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1092" s="8">
-        <f t="shared" si="16"/>
+        <f t="shared" ref="A1092:A1155" si="17">A1091+1</f>
         <v>1090</v>
       </c>
     </row>
     <row r="1093" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1093" s="8">
-        <f t="shared" ref="A1093:A1156" si="17">A1092+1</f>
+        <f t="shared" si="17"/>
         <v>1091</v>
       </c>
     </row>
@@ -10217,13 +10279,13 @@
     </row>
     <row r="1156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1156" s="8">
-        <f t="shared" si="17"/>
+        <f t="shared" ref="A1156:A1219" si="18">A1155+1</f>
         <v>1154</v>
       </c>
     </row>
     <row r="1157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1157" s="8">
-        <f t="shared" ref="A1157:A1220" si="18">A1156+1</f>
+        <f t="shared" si="18"/>
         <v>1155</v>
       </c>
     </row>
@@ -10601,13 +10663,13 @@
     </row>
     <row r="1220" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1220" s="8">
-        <f t="shared" si="18"/>
+        <f t="shared" ref="A1220:A1283" si="19">A1219+1</f>
         <v>1218</v>
       </c>
     </row>
     <row r="1221" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1221" s="8">
-        <f t="shared" ref="A1221:A1284" si="19">A1220+1</f>
+        <f t="shared" si="19"/>
         <v>1219</v>
       </c>
     </row>
@@ -10985,13 +11047,13 @@
     </row>
     <row r="1284" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1284" s="8">
-        <f t="shared" si="19"/>
+        <f t="shared" ref="A1284:A1347" si="20">A1283+1</f>
         <v>1282</v>
       </c>
     </row>
     <row r="1285" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1285" s="8">
-        <f t="shared" ref="A1285:A1348" si="20">A1284+1</f>
+        <f t="shared" si="20"/>
         <v>1283</v>
       </c>
     </row>
@@ -11369,13 +11431,13 @@
     </row>
     <row r="1348" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1348" s="8">
-        <f t="shared" si="20"/>
+        <f t="shared" ref="A1348:A1375" si="21">A1347+1</f>
         <v>1346</v>
       </c>
     </row>
     <row r="1349" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1349" s="8">
-        <f t="shared" ref="A1349:A1376" si="21">A1348+1</f>
+        <f t="shared" si="21"/>
         <v>1347</v>
       </c>
     </row>
@@ -11533,12 +11595,6 @@
       <c r="A1375" s="8">
         <f t="shared" si="21"/>
         <v>1373</v>
-      </c>
-    </row>
-    <row r="1376" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1376" s="8">
-        <f t="shared" si="21"/>
-        <v>1374</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Extra validatie toegevoegd aan toevoegen toeleidingsbegrippen
</commit_message>
<xml_diff>
--- a/catalogusdata/Logische testen Catalogus.xlsx
+++ b/catalogusdata/Logische testen Catalogus.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="235">
   <si>
     <t>US</t>
   </si>
@@ -798,6 +798,15 @@
   </si>
   <si>
     <t>Container geeft als melding "De upload mag geen wijzigingen aanbrengen aan de collectie van toeleidingsbegrippen."</t>
+  </si>
+  <si>
+    <t>Validatie type</t>
+  </si>
+  <si>
+    <t>Concepten/Regressietest/ttl/Validatie type toeleidingsbegrip.ttl</t>
+  </si>
+  <si>
+    <t>Container geeft als resultaat "Een toeleidingsbegrip mag enkel skos:Concept als type hebben."</t>
   </si>
 </sst>
 </file>
@@ -1352,10 +1361,10 @@
   <dimension ref="A1:J1375"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="F84" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="F81" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J92" sqref="J92"/>
+      <selection pane="bottomRight" activeCell="J84" sqref="J84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3958,37 +3967,34 @@
         <v>215</v>
       </c>
     </row>
-    <row r="83" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="8">
         <f t="shared" si="1"/>
         <v>81</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>217</v>
+        <v>232</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>209</v>
       </c>
       <c r="E83" s="7" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="F83" s="8" t="s">
-        <v>219</v>
+        <v>233</v>
       </c>
       <c r="G83" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H83" s="9" t="s">
-        <v>220</v>
-      </c>
       <c r="I83" s="10" t="s">
-        <v>221</v>
+        <v>9</v>
       </c>
       <c r="J83" s="10" t="s">
-        <v>222</v>
+        <v>234</v>
       </c>
     </row>
     <row r="84" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -4000,13 +4006,13 @@
         <v>216</v>
       </c>
       <c r="C84" s="8" t="s">
-        <v>178</v>
+        <v>217</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>209</v>
       </c>
       <c r="E84" s="7" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="F84" s="8" t="s">
         <v>219</v>
@@ -4015,43 +4021,46 @@
         <v>12</v>
       </c>
       <c r="H84" s="9" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="I84" s="10" t="s">
-        <v>85</v>
+        <v>221</v>
       </c>
       <c r="J84" s="10" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A85" s="8">
         <f t="shared" si="1"/>
         <v>83</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>28</v>
+        <v>216</v>
       </c>
       <c r="C85" s="8" t="s">
-        <v>207</v>
+        <v>178</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>209</v>
       </c>
       <c r="E85" s="7" t="s">
-        <v>18</v>
+        <v>223</v>
       </c>
       <c r="F85" s="8" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="G85" s="8" t="s">
         <v>12</v>
       </c>
+      <c r="H85" s="9" t="s">
+        <v>226</v>
+      </c>
       <c r="I85" s="10" t="s">
-        <v>9</v>
+        <v>85</v>
       </c>
       <c r="J85" s="10" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="86" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -4060,7 +4069,7 @@
         <v>84</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C86" s="8" t="s">
         <v>207</v>
@@ -4069,7 +4078,7 @@
         <v>209</v>
       </c>
       <c r="E86" s="7" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="F86" s="8" t="s">
         <v>228</v>
@@ -4090,7 +4099,7 @@
         <v>85</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C87" s="8" t="s">
         <v>207</v>
@@ -4099,16 +4108,13 @@
         <v>209</v>
       </c>
       <c r="E87" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F87" s="8" t="s">
         <v>228</v>
       </c>
       <c r="G87" s="8" t="s">
         <v>12</v>
-      </c>
-      <c r="H87" s="9" t="s">
-        <v>37</v>
       </c>
       <c r="I87" s="10" t="s">
         <v>9</v>
@@ -4123,7 +4129,7 @@
         <v>86</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="C88" s="8" t="s">
         <v>207</v>
@@ -4132,13 +4138,16 @@
         <v>209</v>
       </c>
       <c r="E88" s="7" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="F88" s="8" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G88" s="8" t="s">
         <v>12</v>
+      </c>
+      <c r="H88" s="9" t="s">
+        <v>37</v>
       </c>
       <c r="I88" s="10" t="s">
         <v>9</v>
@@ -4153,7 +4162,7 @@
         <v>87</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C89" s="8" t="s">
         <v>207</v>
@@ -4162,16 +4171,13 @@
         <v>209</v>
       </c>
       <c r="E89" s="7" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F89" s="8" t="s">
         <v>229</v>
       </c>
       <c r="G89" s="8" t="s">
         <v>12</v>
-      </c>
-      <c r="H89" s="9" t="s">
-        <v>37</v>
       </c>
       <c r="I89" s="10" t="s">
         <v>9</v>
@@ -4186,7 +4192,7 @@
         <v>88</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>107</v>
+        <v>69</v>
       </c>
       <c r="C90" s="8" t="s">
         <v>207</v>
@@ -4195,13 +4201,16 @@
         <v>209</v>
       </c>
       <c r="E90" s="7" t="s">
-        <v>109</v>
+        <v>74</v>
       </c>
       <c r="F90" s="8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G90" s="8" t="s">
         <v>12</v>
+      </c>
+      <c r="H90" s="9" t="s">
+        <v>37</v>
       </c>
       <c r="I90" s="10" t="s">
         <v>9</v>
@@ -4216,7 +4225,7 @@
         <v>89</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C91" s="8" t="s">
         <v>207</v>
@@ -4225,16 +4234,13 @@
         <v>209</v>
       </c>
       <c r="E91" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F91" s="8" t="s">
         <v>230</v>
       </c>
       <c r="G91" s="8" t="s">
         <v>12</v>
-      </c>
-      <c r="H91" s="9" t="s">
-        <v>37</v>
       </c>
       <c r="I91" s="10" t="s">
         <v>9</v>
@@ -4249,7 +4255,7 @@
         <v>90</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C92" s="8" t="s">
         <v>207</v>
@@ -4258,7 +4264,7 @@
         <v>209</v>
       </c>
       <c r="E92" s="7" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="F92" s="8" t="s">
         <v>230</v>
@@ -4266,6 +4272,9 @@
       <c r="G92" s="8" t="s">
         <v>12</v>
       </c>
+      <c r="H92" s="9" t="s">
+        <v>37</v>
+      </c>
       <c r="I92" s="10" t="s">
         <v>9</v>
       </c>
@@ -4273,10 +4282,34 @@
         <v>231</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" s="8">
         <f t="shared" si="1"/>
         <v>91</v>
+      </c>
+      <c r="B93" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C93" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E93" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="F93" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="G93" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I93" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="J93" s="10" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Toevoegen regressietesten voor GCO-282
</commit_message>
<xml_diff>
--- a/catalogusdata/Logische testen Catalogus.xlsx
+++ b/catalogusdata/Logische testen Catalogus.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="251">
   <si>
     <t>US</t>
   </si>
@@ -807,6 +807,63 @@
   </si>
   <si>
     <t>Container geeft als resultaat "Een toeleidingsbegrip mag enkel skos:Concept als type hebben."</t>
+  </si>
+  <si>
+    <t>Upload informatiemodel</t>
+  </si>
+  <si>
+    <t>GCO-282</t>
+  </si>
+  <si>
+    <t>container/ttlmodelupload</t>
+  </si>
+  <si>
+    <t>Waardelijsten/Regressietest/Datacontrole informatiemodel.ttl</t>
+  </si>
+  <si>
+    <t>update/createwaardelijst</t>
+  </si>
+  <si>
+    <t>De pagina bevat o.a. een invoerveld met als naam "Selecteer het informatiemodel horende bij de waardelijst" en daarachter de keuzemogelijkheid "Test-Informatiemodel"</t>
+  </si>
+  <si>
+    <t>Aanmaken waardelijst</t>
+  </si>
+  <si>
+    <t>Aanmaken classificerende waardelijst</t>
+  </si>
+  <si>
+    <t>In het scherm wordt het volgende geselecteerd / ingevuld:
+- TestClassificerend
+- Test-Informatiemodel
+- Classificerend</t>
+  </si>
+  <si>
+    <t>Een resultaatpagina verschijnt met daarin drie stappen. Achter 'categoriserend' en 'refererend' staat (o.a.) 'nothing to do' en achter 'classificerend' staat 'done'.</t>
+  </si>
+  <si>
+    <t>Aanmaken categoriserende waardelijst</t>
+  </si>
+  <si>
+    <t>Aanmaken refererende waardelijst</t>
+  </si>
+  <si>
+    <t>In het scherm wordt het volgende geselecteerd / ingevuld:
+- TestCategoriserend
+- Test-Informatiemodel
+- Categoriserend</t>
+  </si>
+  <si>
+    <t>In het scherm wordt het volgende geselecteerd / ingevuld:
+- TestRefererend
+- Test-Informatiemodel
+- Refererend</t>
+  </si>
+  <si>
+    <t>Een resultaatpagina verschijnt met daarin drie stappen. Achter 'classificerend' en 'refererend' staat (o.a.) 'nothing to do' en achter 'categoriserend' staat 'done'.</t>
+  </si>
+  <si>
+    <t>Een resultaatpagina verschijnt met daarin drie stappen. Achter 'categoriserend' en 'classificerend' staat (o.a.) 'nothing to do' en achter 'refererend' staat (o.a.) 'done'.</t>
   </si>
 </sst>
 </file>
@@ -1361,10 +1418,10 @@
   <dimension ref="A1:J1375"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="F81" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="F94" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J84" sqref="J84"/>
+      <selection pane="bottomRight" activeCell="J98" sqref="J98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4312,115 +4369,247 @@
         <v>231</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" s="8">
         <f t="shared" si="1"/>
         <v>92</v>
       </c>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B94" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="C94" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="E94" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="F94" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="G94" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I94" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="J94" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A95" s="8">
         <f t="shared" si="1"/>
         <v>93</v>
       </c>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B95" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="C95" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="E95" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="F95" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="G95" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H95" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="I95" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="J95" s="10" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A96" s="8">
         <f t="shared" si="1"/>
         <v>94</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B96" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="C96" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="E96" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="F96" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="G96" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H96" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="I96" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="J96" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A97" s="8">
         <f t="shared" si="1"/>
         <v>95</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B97" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="C97" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="E97" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="F97" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="G97" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H97" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="I97" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="J97" s="10" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A98" s="8">
         <f t="shared" si="1"/>
         <v>96</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B98" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="C98" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="E98" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="F98" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="G98" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H98" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="I98" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="J98" s="10" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="8">
         <f t="shared" si="1"/>
         <v>97</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="8">
         <f t="shared" si="1"/>
         <v>98</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="8">
         <f t="shared" si="1"/>
         <v>99</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="8">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="8">
         <f t="shared" si="1"/>
         <v>101</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="8">
         <f t="shared" si="1"/>
         <v>102</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="8">
         <f t="shared" si="1"/>
         <v>103</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="8">
         <f t="shared" si="1"/>
         <v>104</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="8">
         <f t="shared" si="1"/>
         <v>105</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="8">
         <f t="shared" si="1"/>
         <v>106</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="8">
         <f t="shared" si="1"/>
         <v>107</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="8">
         <f t="shared" si="1"/>
         <v>108</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="8">
         <f t="shared" si="1"/>
         <v>109</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="8">
         <f t="shared" si="1"/>
         <v>110</v>

</xml_diff>

<commit_message>
Kleine update aan regressietest
</commit_message>
<xml_diff>
--- a/catalogusdata/Logische testen Catalogus.xlsx
+++ b/catalogusdata/Logische testen Catalogus.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="252">
   <si>
     <t>US</t>
   </si>
@@ -864,6 +864,9 @@
   </si>
   <si>
     <t>Een resultaatpagina verschijnt met daarin drie stappen. Achter 'categoriserend' en 'classificerend' staat (o.a.) 'nothing to do' en achter 'refererend' staat (o.a.) 'done'.</t>
+  </si>
+  <si>
+    <t>Testbestand wordt geupload en als naam wordt 'Test' ingevuld</t>
   </si>
 </sst>
 </file>
@@ -1418,10 +1421,10 @@
   <dimension ref="A1:J1375"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="F94" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="D93" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J98" sqref="J98"/>
+      <selection pane="bottomRight" activeCell="I94" sqref="I94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4393,7 +4396,7 @@
         <v>12</v>
       </c>
       <c r="I94" s="10" t="s">
-        <v>9</v>
+        <v>251</v>
       </c>
       <c r="J94" s="10" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Verdere update nav verplaatsing waardelijsten naar /dsov2
</commit_message>
<xml_diff>
--- a/catalogusdata/Logische testen Catalogus.xlsx
+++ b/catalogusdata/Logische testen Catalogus.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="235">
   <si>
     <t>US</t>
   </si>
@@ -807,66 +807,6 @@
   </si>
   <si>
     <t>Container geeft als resultaat "Een toeleidingsbegrip mag enkel skos:Concept als type hebben."</t>
-  </si>
-  <si>
-    <t>Upload informatiemodel</t>
-  </si>
-  <si>
-    <t>GCO-282</t>
-  </si>
-  <si>
-    <t>container/ttlmodelupload</t>
-  </si>
-  <si>
-    <t>Waardelijsten/Regressietest/Datacontrole informatiemodel.ttl</t>
-  </si>
-  <si>
-    <t>update/createwaardelijst</t>
-  </si>
-  <si>
-    <t>De pagina bevat o.a. een invoerveld met als naam "Selecteer het informatiemodel horende bij de waardelijst" en daarachter de keuzemogelijkheid "Test-Informatiemodel"</t>
-  </si>
-  <si>
-    <t>Aanmaken waardelijst</t>
-  </si>
-  <si>
-    <t>Aanmaken classificerende waardelijst</t>
-  </si>
-  <si>
-    <t>In het scherm wordt het volgende geselecteerd / ingevuld:
-- TestClassificerend
-- Test-Informatiemodel
-- Classificerend</t>
-  </si>
-  <si>
-    <t>Een resultaatpagina verschijnt met daarin drie stappen. Achter 'categoriserend' en 'refererend' staat (o.a.) 'nothing to do' en achter 'classificerend' staat 'done'.</t>
-  </si>
-  <si>
-    <t>Aanmaken categoriserende waardelijst</t>
-  </si>
-  <si>
-    <t>Aanmaken refererende waardelijst</t>
-  </si>
-  <si>
-    <t>In het scherm wordt het volgende geselecteerd / ingevuld:
-- TestCategoriserend
-- Test-Informatiemodel
-- Categoriserend</t>
-  </si>
-  <si>
-    <t>In het scherm wordt het volgende geselecteerd / ingevuld:
-- TestRefererend
-- Test-Informatiemodel
-- Refererend</t>
-  </si>
-  <si>
-    <t>Een resultaatpagina verschijnt met daarin drie stappen. Achter 'classificerend' en 'refererend' staat (o.a.) 'nothing to do' en achter 'categoriserend' staat 'done'.</t>
-  </si>
-  <si>
-    <t>Een resultaatpagina verschijnt met daarin drie stappen. Achter 'categoriserend' en 'classificerend' staat (o.a.) 'nothing to do' en achter 'refererend' staat (o.a.) 'done'.</t>
-  </si>
-  <si>
-    <t>Testbestand wordt geupload en als naam wordt 'Test' ingevuld</t>
   </si>
 </sst>
 </file>
@@ -1421,10 +1361,10 @@
   <dimension ref="A1:J1375"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="D93" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B92" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I94" sqref="I94"/>
+      <selection pane="bottomRight" activeCell="B101" sqref="B101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4372,247 +4312,115 @@
         <v>231</v>
       </c>
     </row>
-    <row r="94" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="8">
         <f t="shared" si="1"/>
         <v>92</v>
       </c>
-      <c r="B94" s="8" t="s">
-        <v>235</v>
-      </c>
-      <c r="C94" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D94" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="E94" s="7" t="s">
-        <v>237</v>
-      </c>
-      <c r="F94" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="G94" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="I94" s="10" t="s">
-        <v>251</v>
-      </c>
-      <c r="J94" s="10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="95" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="8">
         <f t="shared" si="1"/>
         <v>93</v>
       </c>
-      <c r="B95" s="8" t="s">
-        <v>235</v>
-      </c>
-      <c r="C95" s="8" t="s">
-        <v>178</v>
-      </c>
-      <c r="D95" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="E95" s="7" t="s">
-        <v>239</v>
-      </c>
-      <c r="F95" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="G95" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H95" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="I95" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="J95" s="10" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="96" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="8">
         <f t="shared" si="1"/>
         <v>94</v>
       </c>
-      <c r="B96" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="C96" s="8" t="s">
-        <v>242</v>
-      </c>
-      <c r="D96" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="E96" s="7" t="s">
-        <v>239</v>
-      </c>
-      <c r="F96" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="G96" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H96" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="I96" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="J96" s="10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="97" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="8">
         <f t="shared" si="1"/>
         <v>95</v>
       </c>
-      <c r="B97" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="C97" s="8" t="s">
-        <v>245</v>
-      </c>
-      <c r="D97" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="E97" s="7" t="s">
-        <v>239</v>
-      </c>
-      <c r="F97" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="G97" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H97" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="I97" s="10" t="s">
-        <v>247</v>
-      </c>
-      <c r="J97" s="10" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="98" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="8">
         <f t="shared" si="1"/>
         <v>96</v>
       </c>
-      <c r="B98" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="C98" s="8" t="s">
-        <v>246</v>
-      </c>
-      <c r="D98" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="E98" s="7" t="s">
-        <v>239</v>
-      </c>
-      <c r="F98" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="G98" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H98" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="I98" s="10" t="s">
-        <v>248</v>
-      </c>
-      <c r="J98" s="10" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="8">
         <f t="shared" si="1"/>
         <v>97</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="8">
         <f t="shared" si="1"/>
         <v>98</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="8">
         <f t="shared" si="1"/>
         <v>99</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="8">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="8">
         <f t="shared" si="1"/>
         <v>101</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="8">
         <f t="shared" si="1"/>
         <v>102</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" s="8">
         <f t="shared" si="1"/>
         <v>103</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="8">
         <f t="shared" si="1"/>
         <v>104</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="8">
         <f t="shared" si="1"/>
         <v>105</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="8">
         <f t="shared" si="1"/>
         <v>106</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="8">
         <f t="shared" si="1"/>
         <v>107</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="8">
         <f t="shared" si="1"/>
         <v>108</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" s="8">
         <f t="shared" si="1"/>
         <v>109</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="8">
         <f t="shared" si="1"/>
         <v>110</v>

</xml_diff>